<commit_message>
Fixbug, create more data
</commit_message>
<xml_diff>
--- a/assets/export/product.xlsx
+++ b/assets/export/product.xlsx
@@ -859,7 +859,7 @@
         <v>78000</v>
       </c>
       <c r="D2">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -877,7 +877,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1019,7 +1019,7 @@
         <v>98000</v>
       </c>
       <c r="D7">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1037,7 +1037,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1307,7 +1307,7 @@
         <v>148000</v>
       </c>
       <c r="D16">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1325,7 +1325,7 @@
         <v>2</v>
       </c>
       <c r="J16">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Salesmanager] Manage Products - Paginate
</commit_message>
<xml_diff>
--- a/assets/export/product.xlsx
+++ b/assets/export/product.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="128">
   <si>
     <t>Mã sản phẩm</t>
   </si>
@@ -470,6 +470,629 @@
   </si>
   <si>
     <t>28/11/2016 16:33</t>
+  </si>
+  <si>
+    <t>Hoa ngọc lan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Theo đ&amp;ocirc;ng y, hoa ngọc lan c&amp;oacute; vị đắng, cay, t&amp;iacute;nh ấm; c&amp;oacute; t&amp;aacute;c dụng d&amp;ugrave;ng để chữa ho, vi&amp;ecirc;m mũi, xoang, tiểu kh&amp;oacute;, đầy hơi, buồn n&amp;ocirc;n, sốt, tăng huyết &amp;aacute;p&amp;hellip; Hoa d&amp;ugrave;ng để l&amp;agrave;m thuốc l&amp;agrave; hoa mới chớm nở, c&amp;oacute; thể d&amp;ugrave;ng ở dạng tươi hoặc kh&amp;ocirc; đều được. D&amp;acirc;n gian thường d&amp;ugrave;ng hoa ngọc lan tẩm mật ong trong 3 ng&amp;agrave;y rồi sắc uống như tr&amp;agrave; để chữa ho, đau đầu, hoa mắt rất tốt.&lt;br /&gt;
+Một số c&amp;aacute;ch d&amp;ugrave;ng hoa Ngọc Lan:&amp;nbsp;&lt;br /&gt;
+1. Chữa đau bụng kinh: Hoa ngọc lan 12g, sắc hoặc h&amp;atilde;m uống thay tr&amp;agrave; v&amp;agrave;o l&amp;uacute;c s&amp;aacute;ng sớm. D&amp;ugrave;ng 30 ng&amp;agrave;y l&amp;agrave; một liệu tr&amp;igrave;nh, c&amp;oacute; t&amp;aacute;c dụng giảm đau bụng kinh ở phụ nữ.&lt;/p&gt;
+&lt;p&gt;2. Chữa v&amp;ocirc; sinh: 10g hoa ngọc lan chưa nở sắc hoặc h&amp;atilde;m uống thay tr&amp;agrave;, v&amp;agrave;o buổi sớm. Cứ 30 ng&amp;agrave;y một liệu tr&amp;igrave;nh, c&amp;oacute; thể cải thiện thống kinh v&amp;agrave; v&amp;ocirc; sinh nữ.&lt;/p&gt;
+&lt;p&gt;3. Chữa ho do lạnh: Hoa ngọc lan 20g, đem tẩmmật ong trong 3 ng&amp;agrave;y rồi sắc uống như tr&amp;agrave;.&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 16:54</t>
+  </si>
+  <si>
+    <t>Kim ngân</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;T&amp;ecirc;n khoa học: Lonicera japonica Thunb, họ Cơm ch&amp;aacute;y(Caprifolianceae).&lt;/p&gt;
+&lt;p&gt;Kim ng&amp;acirc;n c&amp;oacute; Vị đắng, t&amp;iacute;nh h&amp;agrave;n, kh&amp;ocirc;ng độc. C&amp;oacute; t&amp;aacute;c dụng thanh nhiệt, giải độc, v&amp;igrave; vậy được sử dụng để chữa mụn nhọt, r&amp;ocirc;m sảy, thủy đậu, sởi, tả, lỵ, dị ứng&amp;hellip;&lt;/p&gt;
+&lt;p&gt;C&amp;aacute;i T&amp;ecirc;n Kim ng&amp;acirc;n do đặc điểm khi ra hoa của c&amp;acirc;y, những hoa ra sớm sẽ c&amp;oacute; m&amp;agrave;u trắng như bạc, sau 1 thời gian nở c&amp;aacute;c hoa n&amp;agrave;y sẽ chuyển s&amp;agrave;ng m&amp;agrave;u v&amp;agrave;ng. Cho n&amp;ecirc;n tr&amp;ecirc;n c&amp;ugrave;ng một c&amp;acirc;y ta c&amp;oacute; thể thấy cả 2 m&amp;agrave;u sắc hoa c&amp;ugrave;ng hiện diện(kim l&amp;agrave; v&amp;agrave;ng, ng&amp;acirc;n l&amp;agrave; bạc).&lt;/p&gt;
+&lt;p&gt;T&amp;aacute;c dụng dược l&amp;yacute;:&lt;/p&gt;
+&lt;p&gt;1. T&amp;aacute;c dụng kh&amp;aacute;ng khuẩn, kh&amp;aacute;ng virus: ức chế mạnh đối với tụ cầu, thương h&amp;agrave;n, lỵ Shiga&amp;hellip;&lt;br /&gt;
+2. T&amp;aacute;c dụng tăng cường chuyển h&amp;oacute;a Lipid.&lt;br /&gt;
+3. T&amp;aacute;c dụng kh&amp;aacute;ng vi&amp;ecirc;m&lt;br /&gt;
+4. Hưng phấn trung khu thần kinh: =1/6 caf&amp;eacute;.&lt;br /&gt;
+5. Lợi tiểu.&lt;/p&gt;
+&lt;p&gt;C&amp;aacute;ch d&amp;ugrave;ng:&lt;br /&gt;
+Cho một nh&amp;uacute;m Kim ng&amp;acirc;n v&amp;agrave;o ấm, tr&amp;aacute;ng nhanh qua bằng nước s&amp;ocirc;i. Sau đ&amp;oacute; cho tiếp khoảng 200ml nước s&amp;ocirc;i v&amp;agrave;o, đậy nắp khoảng 5 ph&amp;uacute;t l&amp;agrave; được. Khi d&amp;ugrave;ng c&amp;oacute; thể th&amp;ecirc;m chanh, đường, mật ong.&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 16:58</t>
+  </si>
+  <si>
+    <t>Long nhãn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Long nh&amp;atilde;n l&amp;agrave; thực phẩm đ&amp;atilde; qu&amp;aacute; quen thuộc đối với mọi người, c&amp;oacute; thể d&amp;ugrave;ng pha c&amp;ugrave;ng c&amp;agrave;c loại tr&amp;agrave;, hoặc ăn k&amp;egrave;m, hoặc nấu ch&amp;egrave;...&lt;/p&gt;
+&lt;p&gt;T&amp;ecirc;n Long nh&amp;atilde;n xuất ph&amp;aacute;t bởi h&amp;igrave;nh dạng giống mắt của con rồng.&lt;br /&gt;
+S&amp;aacute;ch &amp;ldquo;Thần n&amp;ocirc;ng bản thảo kinh&amp;rdquo; gọi tr&amp;aacute;i nh&amp;atilde;n l&amp;agrave; &amp;ldquo;&amp;Iacute;ch tr&amp;iacute; quả&amp;rdquo;, v&amp;igrave; đ&amp;acirc;y l&amp;agrave; thứ quả c&amp;oacute; t&amp;aacute;c dụng dưỡng huyết &amp;iacute;ch tr&amp;iacute; thần hiệu. Quả nh&amp;atilde;n c&amp;oacute; h&amp;igrave;nh tr&amp;ograve;n n&amp;ecirc;n c&amp;ograve;n c&amp;oacute; t&amp;ecirc;n gọi &amp;ldquo;Quế vi&amp;ecirc;n&amp;rdquo; ( vi&amp;ecirc;n l&amp;agrave; tr&amp;ograve;n), hoặc c&amp;oacute; t&amp;ecirc;n gọi l&amp;agrave; &amp;ldquo;Lệ chi n&amp;ocirc;&amp;rdquo; do m&amp;ugrave;a nh&amp;atilde;n tiếp sau m&amp;ugrave;a vải ( n&amp;ocirc; l&amp;agrave; kẻ theo hầu).&lt;br /&gt;
+Theo Đ&amp;ocirc;ng y, Long nh&amp;atilde;n nhục hay Long nh&amp;atilde;n c&amp;oacute; vị cam, t&amp;iacute;nh &amp;ocirc;n; quy v&amp;agrave;o kinh T&amp;acirc;m v&amp;agrave; Tỳ.&lt;br /&gt;
+C&amp;oacute; t&amp;aacute;c dụng bổ &amp;iacute;ch t&amp;acirc;m tỳ, dưỡng huyết an thần; Chủ trị trống ngực hồi hộp tim loạn nhịp,, mất ngủ hay qu&amp;ecirc;n, k&amp;eacute;m ăn mệt mỏi, đại tiện ra m&amp;aacute;u, phụ nữ băng lậu..&lt;/p&gt;
+&lt;p&gt;Long nh&amp;atilde;n c&amp;oacute; h&amp;agrave;m lượng dinh dưỡng cao, qu&amp;aacute; tr&amp;igrave;nh sấy kh&amp;ocirc; khiến long nh&amp;atilde;n bay hơi gần hết lượng nước. Trong Long nh&amp;atilde;n chứa đường glucose, lipid, vitamin B1,B2,C, P v&amp;agrave; c&amp;aacute;c nguy&amp;ecirc;n tố Canxi, Phospho, sắt..&lt;/p&gt;
+&lt;p&gt;C&amp;aacute;c nghi&amp;ecirc;n cứu dược l&amp;yacute; hiện đại cho thấy, Long nh&amp;atilde;n c&amp;oacute; t&amp;aacute;c dụng chống l&amp;atilde;o suy v&amp;igrave; trong c&amp;ugrave;i c&amp;oacute; Flavoprotein &amp;ndash; một hoạt chất c&amp;oacute; t&amp;aacute;c dụng tăng cường hoạt t&amp;iacute;nh của c&amp;aacute;c tế b&amp;agrave;o thần kinh n&amp;atilde;o.&lt;br /&gt;
+Trong c&amp;ugrave;i nh&amp;atilde;n c&amp;ograve;n c&amp;oacute; Vitamin PP, c&amp;oacute; t&amp;aacute;c dụng l&amp;agrave;m tăng độ bền v&amp;agrave; độ đ&amp;agrave;n hồi của mạch m&amp;aacute;u, gi&amp;uacute;p qu&amp;aacute; tr&amp;igrave;nh tuần ho&amp;agrave;n m&amp;aacute;u tốt hơn.&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:06</t>
+  </si>
+  <si>
+    <t>Bí đao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Bạn thừa c&amp;acirc;n, bạn lo lắng về đ&amp;aacute;m mỡ ở bụng, ở đ&amp;ugrave;i..., bạn đ&amp;atilde; cố nhịn ăn, tập thể dục đến mệt nhừ người...m&amp;agrave; vẫn kh&amp;ocirc;ng ưng &amp;yacute;?&lt;/p&gt;
+&lt;p&gt;B&amp;iacute; đao chư&amp;aacute; nhiều chất xơ, kh&amp;ocirc;ng chứa chất b&amp;eacute;o. Hơn nữa trong b&amp;iacute; đao c&amp;ograve;n chứa hợp chất Hyterin-caperin ngăn kh&amp;ocirc;ng cho đường chuyển ho&amp;aacute; th&amp;agrave;nh mỡ trong cơ thể, n&amp;ecirc;n cơ thể sẽ kh&amp;ocirc;ng bị t&amp;iacute;ch luỹ mỡ thừa.&lt;/p&gt;
+&lt;p&gt;Ngo&amp;agrave;i ra trong b&amp;iacute; đao chứa nhiều c&amp;aacute;c vitamin C, vitamin E, v&amp;agrave; c&amp;aacute;c kho&amp;aacute;ng chất Kali, Phospho, Magie&amp;hellip; gi&amp;uacute;p l&amp;agrave;m đẹp cơ thể. B&amp;iacute; đao vốn l&amp;agrave; một phương thuốc l&amp;agrave;m đẹp của c&amp;aacute;c mỹ nh&amp;acirc;n được lưu truyền từ xưa, n&amp;oacute; giữ ẩm cho da, l&amp;agrave;m da căng mịn, s&amp;aacute;ng hồng, bớt dầu v&amp;agrave; mụn đầu đen.&lt;/p&gt;
+&lt;p&gt;Chỉ cần cho b&amp;iacute; đao v&amp;agrave;o nước ấm để h&amp;atilde;m lấy nước uống thay nước lọc trong ng&amp;agrave;y. Trong 1 th&amp;aacute;ng bạn sẽ thấy v&amp;oacute;c d&amp;aacute;ng cơ thể được cải thiện r&amp;otilde; rệt&amp;nbsp;&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:08</t>
+  </si>
+  <si>
+    <t>Trà Atiso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h3&gt;T&amp;aacute;c dụng của tr&amp;agrave; atiso&lt;/h3&gt;
+&lt;p&gt;&amp;nbsp;Tr&amp;agrave; aitso kh&amp;ocirc;ng những t&amp;aacute;c dụng giảm c&amp;acirc;n c&amp;ograve;n tốt cho t&amp;oacute;c, đẹp da, giải độc m&amp;aacute;t gan, giữ g&amp;igrave;n tuổi thanh xu&amp;acirc;n cho phụ nữ v&amp;agrave; đặc biệt đem lại v&amp;ograve;ng eo thon gọn.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Bạn c&amp;oacute; thể t&amp;igrave;m đến c&amp;aacute;c loại tr&amp;agrave; atiso đ&amp;atilde; đ&amp;oacute;ng g&amp;oacute;i tr&amp;ecirc;n thị trường, t&amp;igrave;m v&amp;agrave; chọn mua cho m&amp;igrave;nh tr&amp;agrave; atiso th&amp;iacute;ch hợp để giảm c&amp;acirc;n cũng như tốt cho sức khỏe.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;C&amp;aacute;ch uống tr&amp;agrave; atiso giảm c&amp;acirc;n hiệu quả&lt;/h3&gt;
+&lt;p&gt;Để giảm c&amp;acirc;n hiệu quả c&amp;ugrave;ng tr&amp;agrave; atiso, bạn phải tu&amp;acirc;n thủ một v&amp;agrave;i nguy&amp;ecirc;n tắc sau đ&amp;acirc;y :&lt;/p&gt;
+&lt;p&gt;Uống đ&amp;ecirc;u đặn mỗi ng&amp;agrave;y mới ph&amp;aacute;t huy được c&amp;ocirc;ng dụng hiệu quả của atiso&lt;/p&gt;
+&lt;p&gt;N&amp;ecirc;n bảo quản tr&amp;agrave; trong thời gian ngắn, tốt nhất l&amp;agrave; pha v&amp;agrave; uống trong ng&amp;agrave;y, để tr&amp;aacute;nh tr&amp;agrave; bị thi&amp;ecirc;u&lt;/p&gt;
+&lt;p&gt;Nếu bạn kh&amp;oacute; ngủ, kh&amp;ocirc;ng n&amp;ecirc;n uống tr&amp;agrave; sau 16h, kh&amp;ocirc;ng uống qu&amp;aacute; 1 ly tr&amp;agrave;/ ng&amp;agrave;y&lt;/p&gt;
+&lt;p&gt;C&amp;oacute; thể uống tr&amp;agrave; v&amp;agrave;o buổi s&amp;aacute;ng thay cho c&amp;agrave; ph&amp;ecirc; để gi&amp;uacute;p bạn tiết kiệm calo. Uống c&amp;agrave; ph&amp;ecirc; nhiều đường sẽ l&amp;agrave;m bạn tăng c&amp;acirc;n,&lt;/p&gt;
+&lt;p&gt;Nếu bạn kh&amp;ocirc;ng tăng c&amp;acirc;n vẫn c&amp;oacute; thể sử dụng tr&amp;agrave; atiso để tăng cường sức khỏe, đẹp da.&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:11</t>
+  </si>
+  <si>
+    <t>Cỏ ngọt sấy khô</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h3&gt;Đặc điểm&lt;/h3&gt;
+&lt;p&gt;L&amp;agrave; một loại cỏ sống l&amp;acirc;u năm, 6 th&amp;aacute;ng sau khi trồng; gốc bắt đầu ho&amp;aacute; gỗ, mỗi gốc c&amp;oacute; nhiều c&amp;agrave;nh (nếu để mọc tự nhi&amp;ecirc;n c&amp;acirc;y c&amp;oacute; thể cao đến 100cm). C&amp;agrave;nh non v&amp;agrave; l&amp;aacute; đều phủ l&amp;ocirc;ng trắng mịn, l&amp;aacute; mọc đối, h&amp;igrave;nh mũi m&amp;aacute;c, d&amp;agrave;i 30-60mm, rộng 15-30mm, c&amp;oacute; 3 g&amp;acirc;n ch&amp;iacute;nh xuất ph&amp;aacute;t từ cuống l&amp;aacute;. M&amp;eacute;p l&amp;aacute; c&amp;oacute; răng cưa ở nửa phần tr&amp;ecirc;n. Cụm hoa h&amp;igrave;nh đầu, mỗi tổng bao c&amp;oacute; chứa 5 hoa nhỏ, tr&amp;agrave;ng h&amp;igrave;nh ống, m&amp;agrave;u trắng ng&amp;agrave;, c&amp;oacute; 5 c&amp;aacute;nh nhỏ. Hoa d&amp;agrave;i 10-12mm. C&amp;oacute; hai v&amp;ograve;i nhuỵ d&amp;agrave;i th&amp;ograve; ra ngo&amp;agrave;i. Hoa c&amp;oacute; m&amp;ugrave;i thơm nhẹ (h&amp;igrave;nh d&amp;aacute;ng giống hoa cỏ L&amp;agrave;o, nhưng nhỏ hơn nhiều). M&amp;ugrave;a hoa từ th&amp;aacute;ng 10 năm trước đến th&amp;aacute;ng 2 năm sau (theo dương lịch).&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;To&amp;agrave;n th&amp;acirc;n c&amp;oacute; vị ngọt, nhiều nhất ở l&amp;aacute;, l&amp;aacute; gi&amp;agrave; chết kh&amp;ocirc; ở dưới nhưng cuống rất dai n&amp;ecirc;n kh&amp;ocirc;ng rụng (vẫn c&amp;ograve;n vị ngọt).&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Cỏ ngọt sinh sản hữu t&amp;iacute;nh (gieo hạt) v&amp;agrave; v&amp;ocirc; t&amp;iacute;nh (gi&amp;acirc;m c&amp;agrave;nh) l&amp;agrave; c&amp;acirc;y ưa ẩm, ưa s&amp;aacute;ng nhưng sợ &amp;uacute;ng v&amp;agrave; chết khi ngập nước.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Bộ phận d&amp;ugrave;ng: c&amp;agrave;nh mang l&amp;aacute; phơi hoặc sấy kh&amp;ocirc; (Khi đoạn c&amp;agrave;nh d&amp;agrave;i khoảng 20-25cm l&amp;agrave; thời điểm cắt c&amp;agrave;nh. Trung b&amp;igrave;nh mỗi th&amp;aacute;ng một lần thu hoạch)&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Hoạt chất ch&amp;iacute;nh: Steviosid (l&amp;agrave; một glucosid) c&amp;oacute; vị ngọt gấp 250-300 lần đường k&amp;iacute;nh (saccharoza), nhưng stevioside kh&amp;ocirc;ng sinh năng lượng. Trong Cỏ ngọt kh&amp;ocirc; (cả c&amp;agrave;nh l&amp;aacute;) chứa khoảng 1,5% chất ngọt steviosid (trong l&amp;aacute; chứa khoảng 6-7% steviosid). Như vậy 100g Cỏ ngọt kh&amp;ocirc; c&amp;oacute; lượng chất ngọt tương đương 400-450g đường k&amp;iacute;nh.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Tr&amp;ecirc;n thị trường c&amp;oacute; đường Cỏ ngọt dập vi&amp;ecirc;n, mỗi vi&amp;ecirc;n c&amp;oacute; 60mg steviosid tương đương 18g đường k&amp;iacute;nh. Đường cỏ ngọt d&amp;ugrave;ng để pha nước uống như nước chanh, c&amp;agrave; ph&amp;ecirc;...&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;T&amp;aacute;c dụng chữa bệnh: Cỏ ngọt v&amp;agrave; đường Cỏ ngọt kh&amp;ocirc;ng c&amp;oacute; t&amp;aacute;c dụng chữa bệnh m&amp;agrave; l&amp;agrave; chất tạo vị ngọt (kh&amp;ocirc;ng năng lượng) d&amp;ugrave;ng cho:&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;- Người bệnh phải ki&amp;ecirc;ng đường k&amp;iacute;nh (saccharoza) l&amp;agrave; chất sinh năng lượng trong c&amp;aacute;c bệnh như &amp;nbsp;tiểu đường, cắt dạ d&amp;agrave;y, b&amp;eacute;o ph&amp;igrave; cần giảm c&amp;acirc;n&amp;hellip;&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;- C&amp;aacute;c trường hợp phải ki&amp;ecirc;ng d&amp;ugrave;ng Cam thảo Bắc: người mang thai, người c&amp;oacute; bệnh tim mạch, cao huyết &amp;aacute;p. Người đang d&amp;ugrave;ng thuốc c&amp;oacute; Digitalis, thuốc lợi tiểu nh&amp;oacute;m thiazid (v&amp;iacute; dụ uống tr&amp;agrave; nh&amp;acirc;n trần phải bỏ Cam thảo Bắc, thay bằng Cỏ ngọt...)&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;C&amp;aacute;ch d&amp;ugrave;ng&lt;/h3&gt;
+&lt;p&gt;Nếu ngửi thấy c&amp;oacute; m&amp;ugrave;i ng&amp;aacute;i, cần khử m&amp;ugrave;i ng&amp;aacute;i; phơi sấy kh&amp;ocirc;, cắt nhỏ Cỏ ngọt để phối hợp với loại thuốc cần tạo vị ngọt.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;V&amp;iacute; dụ: Hoa ho&amp;egrave;, Nh&amp;acirc;n trần, Actis&amp;ocirc;... khi pha tr&amp;agrave; hoặc sắc thuốc.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Liều lượng: Tuỳ khẩu vị từng người m&amp;agrave; điều chỉnh lượng Cỏ ngọt cho vừa miệng.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;C&amp;aacute;ch khử m&amp;ugrave;i ng&amp;aacute;i: Cỏ ngọt mới l&amp;agrave;m kh&amp;ocirc; sau thu hoạch thường c&amp;oacute; m&amp;ugrave;i ng&amp;aacute;i, g&amp;acirc;y kh&amp;oacute; chịu cho một số người. &amp;nbsp;C&amp;aacute;ch l&amp;agrave;m như sau: Phun nước v&amp;agrave;o Cỏ ngọt kh&amp;ocirc; để l&amp;agrave;m ẩm đều. Cho v&amp;agrave;o t&amp;uacute;i k&amp;iacute;n, ủ trong 2-3 ng&amp;agrave;y rồi đem phơi hoặc sấy kh&amp;ocirc; sẽ hết m&amp;ugrave;i ng&amp;aacute;i m&amp;agrave; kh&amp;ocirc;ng giảm độ ngọt.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Bảo quản: Phơi hoặc sấy kh&amp;ocirc; rồi bảo quản trong đồ đựng sạch, kh&amp;ocirc;, k&amp;iacute;n. Ch&amp;uacute; &amp;yacute; ph&amp;ograve;ng ẩm, mốc.&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:13</t>
+  </si>
+  <si>
+    <t>Trà Tâm Lan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;strong&gt;Chức năng:&lt;/strong&gt;&lt;br /&gt;
+&lt;br /&gt;
+- T&amp;aacute;c dụng thanh nhiệt, giải độc, giải kh&amp;aacute;t&lt;br /&gt;
+&lt;br /&gt;
+- T&amp;aacute;c dụng giảm thiểu nguy cơ rối loạn ti&amp;ecirc;u h&amp;oacute;a, lo&amp;eacute;t dạ d&amp;agrave;y, t&amp;aacute; tr&amp;agrave;ng, đại tr&amp;agrave;ng.&lt;br /&gt;
+&lt;br /&gt;
+- T&amp;aacute;c dụng chống oxy h&amp;oacute;a, hỗ trợ điều trị khối u, ( u tử cung, u v&amp;uacute;, tiền liệt tuyến....). Cao huyết &amp;aacute;p, tăng mỡ m&amp;aacute;u, đường m&amp;aacute;u v&amp;agrave; hỗ trợ an thần, tăng sức bền th&amp;agrave;nh mạch,.&lt;br /&gt;
+&lt;br /&gt;
+- T&amp;aacute;c dụng hỗ trợ tăng sức đề kh&amp;aacute;ng, khả năng miễn dịch, hỗ trợ chống dị ứng.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Th&amp;agrave;nh phần:&lt;/strong&gt;&lt;br /&gt;
+&lt;br /&gt;
+- C&amp;acirc;y ho&amp;agrave;n ngọc (rễ, th&amp;acirc;n, l&amp;aacute;) 40%, C&amp;uacute;c hoa 20%, Kim ng&amp;acirc;n hoa 20%, C&amp;acirc;y lược v&amp;agrave;ng 20%&lt;br /&gt;
+&lt;br /&gt;
+&lt;strong&gt;C&amp;aacute;ch d&amp;ugrave;ng:&lt;/strong&gt;&lt;br /&gt;
+&lt;br /&gt;
+- C&amp;aacute;ch 1: mỗi lần cho 1 t&amp;uacute;i tr&amp;agrave; h&amp;atilde;m v&amp;agrave;o cốc nước s&amp;ocirc;i, sau 3&amp;gt;5 ph&amp;uacute;t l&amp;agrave; uống được&lt;br /&gt;
+&lt;br /&gt;
+- C&amp;aacute;ch 2: cho 2 t&amp;uacute;i lọc v&amp;agrave;o b&amp;igrave;nh đun s&amp;ocirc;i từ 10&amp;gt;15 ph&amp;uacute;t l&amp;agrave; d&amp;ugrave;ng được, c&amp;oacute; thể uống thay nước h&amp;agrave;ng ng&amp;agrave;y.&lt;br /&gt;
+&lt;br /&gt;
+Khối lượng: 120g/ hộp (30 t&amp;uacute;i x 4g)&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:14</t>
+  </si>
+  <si>
+    <t>Trà cung đình Huế</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;strong&gt;C&amp;ocirc;ng dụng của Tr&amp;agrave;&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Trong th&amp;agrave;nh phần của Tr&amp;agrave; Cung Đ&amp;igrave;nh Huế bao gồm rất nhiều loại thảo dược,v&amp;iacute; như: Atis&amp;ocirc;, C&amp;uacute;c hoa, Cỏ ngọt, Ho&amp;agrave;i sơn, Đẳng s&amp;acirc;m, Đại t&amp;aacute;o, Hồng t&amp;aacute;o,Hồi hoa, Cam thảo Bắc, Hoa l&amp;agrave;i, Hoa h&amp;ograve;e, Thảo quyết minh, Khổ qua, Kỷtử, Vối nụ, Tim sen. Mỗi vi thảo dược c&amp;oacute; một chức năng một c&amp;ocirc;ng dụngri&amp;ecirc;ng, t&amp;aacute;c dụng đến từng bộ phận của cơ thể. Khi tinh chế lại với nhautheo một b&amp;iacute; quyết gia truyền sẽ tạo ra một sản phẩm độc nhất v&amp;ocirc; nhị vềc&amp;ocirc;ng dụng, bao gồm:&lt;br /&gt;
+* Hỗ trợ điều trị chứng cao huyết &amp;aacute;p, đau đầu, tim hồi hộp, mất ngủ.&lt;br /&gt;
+* Gi&amp;uacute;p tăng cường sức đề kh&amp;aacute;ng, giảm cholestorol.&lt;br /&gt;
+* Bổ khi huyết, thanh nhiệt, giảm độc, m&amp;aacute;t gan, đẹp da, hết mụn.&lt;br /&gt;
+Ngo&amp;agrave;i ra, sản phẩm n&amp;agrave;y c&amp;ograve;n tốt cho những người mắt yếu, tiểu đường, sỏi thận. Đặc biệt rất th&amp;iacute;ch hợp với phụ nữ.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;C&amp;Aacute;CH THƯỞNG THỨC&lt;/strong&gt;:&amp;nbsp; Trộnđều g&amp;oacute;i tr&amp;agrave;, cho 30g Tr&amp;agrave; th&amp;ecirc;m 2-3 tr&amp;aacute;i t&amp;aacute;o v&amp;agrave;o b&amp;igrave;nh, đổ nước s&amp;ocirc;i, tr&amp;aacute;ngnước đầu. Ch&amp;acirc;m nước s&amp;ocirc;i v&amp;agrave;o, 5 ph&amp;uacute;t sau sẽ cho ra một b&amp;igrave;nh Tr&amp;agrave; CungĐ&amp;igrave;nh Nhất Dạ Đế Vương để thưởng thức. C&amp;oacute; thể bỏ ấm nấu s&amp;ocirc;i, để nguội,đ&amp;oacute;ng chai, bỏ tủ lạnh uống h&amp;agrave;ng ng&amp;agrave;y, m&amp;ugrave;a h&amp;egrave; th&amp;ecirc;m đ&amp;aacute;.&lt;br /&gt;
+&lt;strong&gt;BẢO QUẢN&lt;/strong&gt;: Để Tr&amp;agrave; nơi kh&amp;ocirc; r&amp;aacute;o, tho&amp;aacute;ng m&amp;aacute;t.&lt;/p&gt;
+&lt;p&gt;Danh tr&amp;agrave; Đức Phượng xin c&amp;oacute; đ&amp;ocirc;i lời t&amp;acirc;mgiao: Trải qua bao thăng trầm của thời gian, mỗi ch&amp;uacute;ng ta ai cũng trảiqua một lần uống một ly tr&amp;agrave; n&amp;oacute;ng hoặc lạnh. Ng&amp;agrave;y xưa c&amp;oacute; tr&amp;agrave; Bắc Th&amp;aacute;i,tr&amp;agrave; m&amp;oacute;c c&amp;acirc;u, tr&amp;agrave; sen, tr&amp;agrave; l&amp;agrave;i. Mỗi loại tr&amp;agrave; c&amp;oacute; một đặc t&amp;iacute;nh ri&amp;ecirc;ng củan&amp;oacute;. Tr&amp;agrave; Bắc Th&amp;aacute;i, tr&amp;agrave; m&amp;oacute;c c&amp;acirc;u khi uống v&amp;ocirc; th&amp;igrave; kh&amp;oacute; ngủ. Tr&amp;agrave; ướp xen ướpl&amp;agrave;i uống v&amp;ocirc;, hương vị đ&amp;acirc;u phải l&amp;agrave; hương tự nhi&amp;ecirc;n, nếu c&amp;oacute; th&amp;igrave; rất &amp;iacute;t. V&amp;agrave;ng&amp;agrave;y nay, khi tr&amp;agrave; t&amp;uacute;i lọc ra đời th&amp;igrave; ta đ&amp;acirc;u c&amp;oacute; thể quan s&amp;aacute;t được đ&amp;oacute; l&amp;agrave;nguy&amp;ecirc;n liệu g&amp;igrave; m&amp;agrave; người ta say ra.&lt;br /&gt;
+C&amp;ograve;n b&amp;acirc;y giờ, nếu bạn pha một b&amp;igrave;nh Tr&amp;agrave; Cung Đ&amp;igrave;nh v&amp;agrave;o một b&amp;igrave;nh thuỷ tinh,khi đ&amp;oacute; bạn sẽ cảm thấy r&amp;otilde; r&amp;agrave;ng c&amp;aacute;i tinh hoa của n&amp;oacute;. Những b&amp;ocirc;ng hoa c&amp;uacute;c,hoa l&amp;agrave;i xo&amp;egrave; nở, những tr&amp;aacute;i hồng t&amp;aacute;o, đại t&amp;aacute;o khoe m&amp;agrave;u v&amp;agrave; khi thưởng thứcc&amp;aacute;i vị ngọt lịm thanh tao nơi đầu m&amp;ocirc;i ch&amp;oacute;t lưỡi. &amp;Ocirc;i tuyệt vời l&amp;agrave;m sao!&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:16</t>
+  </si>
+  <si>
+    <t>Nụ vối Hải Hậu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Bạn c&amp;oacute; biết nụ vối , l&amp;aacute; vối những sản phẩm cực k&amp;igrave; gần gũi gắn liền với cuộc sống ch&amp;uacute;ng ta .Đặc biệt đối với c&amp;aacute;c bạn ở l&amp;agrave;ng qu&amp;ecirc;.Nhưng kh&amp;ocirc;ng hẳn ch&amp;uacute;ng ta đều biết t&amp;aacute;c dụng của sản phẩm n&amp;agrave;y. V&amp;agrave; Đặc biệt đối với sức khỏe con người :&lt;br /&gt;
+&lt;br /&gt;
++ &amp;quot;Thần dược&amp;quot; cho bệnh ti&amp;ecirc;u h&amp;oacute;a&lt;br /&gt;
++Ph&amp;ograve;ng v&amp;agrave; điều trị tiểu đường nhờ nụ vối&lt;br /&gt;
++Chống &amp;ocirc; xy h&amp;oacute;a cho cơ thể&lt;br /&gt;
++Gi&amp;uacute;p đ&amp;agrave;o thải chất độc&lt;br /&gt;
++Thuốc s&amp;aacute;t khuẩn cho da&lt;br /&gt;
+C&amp;aacute;ch sử dụng rất đơn giản:&lt;br /&gt;
+L&amp;aacute; vối kh&amp;ocirc; rửa sạch cho v&amp;agrave;o ấm, cho nước lạnh v&amp;agrave;o đun đến s&amp;ocirc;i rồi uống n&amp;oacute;ng hoặc uống lạnh. Nụ vối cũng được đun trong nước đến khi s&amp;ocirc;i hoặc, h&amp;atilde;m trong nước s&amp;ocirc;i như c&amp;aacute;ch h&amp;atilde;m tr&amp;agrave; xanh.&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:17</t>
+  </si>
+  <si>
+    <t>Bí ngô</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;strong&gt;1. T&amp;ecirc;n khoa học:&amp;nbsp;&lt;/strong&gt;Cucurbita pepo L.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;2. Họ:&lt;/strong&gt;&amp;nbsp;Bầu b&amp;iacute; (Cucurbitaceae).&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;3. T&amp;ecirc;n kh&amp;aacute;c:&lt;/strong&gt;&amp;nbsp;B&amp;iacute; đỏ, B&amp;ugrave; rợ.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;4. M&amp;ocirc; tả:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;C&amp;acirc;y thảo, sống l&amp;acirc;u năm. Th&amp;acirc;n c&amp;oacute; năm cạnh, c&amp;oacute; l&amp;ocirc;ng dầy, thường c&amp;oacute; rễ ở những đốt. L&amp;aacute; mọc so le, c&amp;oacute; cuống d&amp;agrave;i 8-20 cm, phiến l&amp;aacute; mềm, h&amp;igrave;nh trứng rộng hoặc gần tr&amp;ograve;n, chia th&amp;ugrave;y n&amp;ocirc;ng, đầu tr&amp;ograve;n hoặc hơi nhọn, m&amp;eacute;p c&amp;oacute; răng cưa, hai mặt l&amp;aacute; c&amp;oacute; nhiều l&amp;ocirc;ng mềm, đ&amp;ocirc;i khi c&amp;oacute; những đốm trắng ở mặt tr&amp;ecirc;n ; tua cuốn ph&amp;acirc;n nh&amp;aacute;nh. Hoa đơn t&amp;iacute;nh c&amp;ugrave;ng gốc, mầu v&amp;agrave;ng ; hoa đực c&amp;oacute; đế hoa ngắn ; đ&amp;agrave;i loe rộng c&amp;oacute; th&amp;ugrave;y h&amp;igrave;nh dải hoặc gần dạng l&amp;aacute;, tr&amp;agrave;ng hoa c&amp;oacute; 5 th&amp;ugrave;y rộng ; hoa c&amp;aacute;i c&amp;oacute; l&amp;aacute; đ&amp;agrave;i dạng l&amp;aacute; r&amp;otilde;,&amp;nbsp; bầu h&amp;igrave;nh tr&amp;ograve;n hoặc hơi d&amp;agrave;i. Quả to, c&amp;ugrave;i d&amp;agrave;y, rỗng giữa c&amp;oacute; nhiều dạng : dạng tr&amp;ograve;n, hơi dẹt, c&amp;oacute; r&amp;atilde;nh s&amp;acirc;u ; dạng h&amp;igrave;nh trứng hoặc h&amp;igrave;nh trứng hơi d&amp;agrave;i, c&amp;oacute; kh&amp;iacute;a r&amp;atilde;nh, vỏ ngo&amp;agrave;i nhẵn, khi ch&amp;iacute;n mầu v&amp;agrave;ng trắng, vỏ giữa mầu v&amp;agrave;ng cam, c&amp;oacute; m&amp;ugrave;i thơm, vị ngọt lợ, cuống quả c&amp;oacute; r&amp;atilde;nh v&amp;agrave; loe rộng ở chỗ tiếp gi&amp;aacute;p với quả ; hạt mầu trắng x&amp;aacute;m, c&amp;oacute; m&amp;eacute;p mỏng v&amp;agrave; mầu sẫm hơn. M&amp;ugrave;a hoa : th&amp;aacute;ng 3-4 ; m&amp;ugrave;a quả th&amp;aacute;ng 5-6&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;5. Ph&amp;acirc;n bố:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;C&amp;acirc;y được trồng nhiều nơi l&amp;agrave;m thực phẩm.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;6. Trồng trọt:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;C&amp;aacute;c v&amp;ugrave;ng chuy&amp;ecirc;n canh&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;7. Bộ phận d&amp;ugrave;ng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Hạt quả b&amp;iacute; ng&amp;ocirc; đ&amp;atilde; gi&amp;agrave;, ch&amp;iacute;n v&amp;agrave; đ&amp;atilde; chế biến kh&amp;ocirc; (Semen Cucurbitae).&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;8. Thu h&amp;aacute;i, chế biến:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Khi c&amp;acirc;y được 2-3 l&amp;aacute; ch&amp;iacute;nh thức, cắt ngọn, mỗi nh&amp;aacute;nh n&amp;ecirc;n giữ 2-3 quả để c&amp;oacute; quả to, cắt bỏ phần ngọn sau quả thứ 3. &amp;ETH;ể l&amp;agrave;m rau ăn, c&amp;oacute; thể d&amp;ugrave;ng quả non hay quả gi&amp;agrave;. &amp;ETH;ể l&amp;agrave;m thuốc, ta thu h&amp;aacute;i quả gi&amp;agrave;, lấy thịt quả d&amp;ugrave;ng tươi, c&amp;ograve;n hạt c&amp;oacute; thể d&amp;ugrave;ng tươi hay phơi kh&amp;ocirc; d&amp;ugrave;ng dần.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;9. Th&amp;agrave;nh phần ho&amp;aacute; học:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Hạt b&amp;iacute; ng&amp;ocirc; c&amp;oacute; c&amp;aacute;c chất protid, lipid, glucid, c&amp;aacute;c chất kho&amp;aacute;ng P, Mg, Ca, K. Hoạt chất l&amp;agrave; một alcaloid: cucurbitin trong ph&amp;ocirc;i v&amp;agrave; vỏ lụa (c&amp;oacute; t&amp;aacute;c dụng tẩy giun s&amp;aacute;n).&lt;br /&gt;
+C&amp;ugrave;i quả b&amp;iacute; ng&amp;ocirc; c&amp;oacute; c&amp;aacute;c chất protid, lipid, glucid, c&amp;aacute;c acid amin (arginin, adenin&amp;hellip;) c&amp;aacute;c chất kho&amp;aacute;ng P, Na, K, Ca, Mg, Fe, Cu, As,&amp;hellip; c&amp;aacute;c vitamin B1, C, caroten.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;10. C&amp;ocirc;ng năng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Tẩy giun s&amp;aacute;n, ức chế sự ph&amp;aacute;t triển của s&amp;aacute;n m&amp;aacute;ng c&amp;ograve;n gọi Huyết hấp tr&amp;ugrave;ng (schistosomiase). C&amp;ugrave;i quả b&amp;iacute; ng&amp;ocirc; được coi như c&amp;oacute; t&amp;aacute;c dụng bổ n&amp;atilde;o.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;11. C&amp;ocirc;ng dụng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Chữa s&amp;aacute;n.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;12. C&amp;aacute;ch d&amp;ugrave;ng, liều lượng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;B&amp;oacute;c hết vỏ cứng, để nguy&amp;ecirc;n m&amp;agrave;ng xanh ở trong, gi&amp;atilde; nhỏ trộn với đường hoặc mật để ăn v&amp;agrave;o l&amp;uacute;c đ&amp;oacute;i, sau khoảng 3 giờ uống thuốc tẩy muối, đi ngo&amp;agrave;i trong một chậu nước ấm. Người lớn d&amp;ugrave;ng khoảng 100g nh&amp;acirc;n hạt. Trẻ con 3-4 tuổi d&amp;ugrave;ng 30g; 5-10 tuổi d&amp;ugrave;ng 75g.&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:19</t>
+  </si>
+  <si>
+    <t>Bách hợp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;strong&gt;1. T&amp;ecirc;n khoa học:&amp;nbsp;&lt;/strong&gt;Lilium brownii var. colchester Wils.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;2. Họ:&lt;/strong&gt;&amp;nbsp;H&amp;agrave;nh (Liliaceae)&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;3. T&amp;ecirc;n kh&amp;aacute;c:&lt;/strong&gt;&amp;nbsp;C&amp;aacute;nh hoa li ly&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;4. M&amp;ocirc; tả:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;C&amp;acirc;y thảo cao 0,5-1m, sống nhiều năm. Th&amp;acirc;n h&amp;agrave;nh to m&amp;agrave;u trắng đục c&amp;oacute; khi phớt hồng, gần h&amp;igrave;nh cầu, vẩy nhẵn v&amp;agrave; dễ gẫy. L&amp;aacute; mọc so le, h&amp;igrave;nh mắc thu&amp;ocirc;n, m&amp;eacute;p nguy&amp;ecirc;n, d&amp;agrave;i 2-15cm, rộng 0,5-3,5cm. Cụm hoa mọc ở đầu c&amp;agrave;nh, gồm 2-6 hoa to, h&amp;igrave;nh loa k&amp;egrave;n, d&amp;agrave;i 14-16cm, với 6 c&amp;aacute;nh hoa m&amp;agrave;u trắng hay hơi hồng. Quả nang 5-6cm c&amp;oacute; 3 ngăn, chứa nhiều hạt nhỏ h&amp;igrave;nh tr&amp;aacute;i xoan.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;5. Ph&amp;acirc;n bố:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;C&amp;acirc;y B&amp;aacute;ch hợp&amp;nbsp; mọc hoang ở một số v&amp;ugrave;ng n&amp;uacute;i cao nước ta. Vị thuốc chủ yếu nhập từ Trung Quốc.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;6. Trồng trọt:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;7. Bộ phận d&amp;ugrave;ng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Vẩy đ&amp;atilde; chế biến kh&amp;ocirc; của c&amp;acirc;y B&amp;aacute;ch hợp (Lilium brownii var. colchester Wils.), họ H&amp;agrave;nh (Liliaceae).&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;8. Thu h&amp;aacute;i, chế biến:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Sau một năm thu hoạch thường người ta ngắt hết hoa để cho củ to. Thu hoạch củ v&amp;agrave;o cuối m&amp;ugrave;a h&amp;egrave;, đầu thu, khi c&amp;acirc;y bắt đầu kh&amp;ocirc; h&amp;eacute;o. &amp;ETH;&amp;agrave;o về rửa sạch, t&amp;aacute;ch ri&amp;ecirc;ng từng vẩy, nh&amp;uacute;ng nước s&amp;ocirc;i 5-10 ph&amp;uacute;t cho vừa ch&amp;iacute;n t&amp;aacute;i, rồi đem phơi hay sấy kh&amp;ocirc;.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;9. Th&amp;agrave;nh phần ho&amp;aacute; học:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Tinh bột (30%), protid (4%), lipid (0,1%), vitamin C, alcaloid.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;10. C&amp;ocirc;ng năng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Nhuận phế, giảm ho, định t&amp;acirc;m, kiện vị, dưỡng trung ti&amp;ecirc;u&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;11. C&amp;ocirc;ng dụng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Chữa ho nhiều do lao, thổ huyết, mệt mỏi, hồi hộp.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;12. C&amp;aacute;ch d&amp;ugrave;ng, liều lượng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Ng&amp;agrave;y d&amp;ugrave;ng 8-20g dạng thuốc sắc hoặc bột. Phối hợp trong c&amp;aacute;c phương thuốc bổ phế chỉ kh&amp;aacute;i, ho lao suy nhược. Dạng thuốc sắc hoặc ho&amp;agrave;n, t&amp;aacute;n.&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:20</t>
+  </si>
+  <si>
+    <t>Bạch đậu khấu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;strong&gt;1. T&amp;ecirc;n khoa học:&amp;nbsp;&lt;/strong&gt;Amomum cardamomum L.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;2. Họ:&lt;/strong&gt;&amp;nbsp;Gừng (Zingiberaceae).&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;3. T&amp;ecirc;n kh&amp;aacute;c:&amp;nbsp;&lt;/strong&gt;Đậu khấu, vi&amp;ecirc;n đậu khấu&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;4. M&amp;ocirc; tả:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;C&amp;acirc;y: C&amp;acirc;y thảo cao khoảng 2-3m. Th&amp;acirc;n rễ nằm ngang to bằng ng&amp;oacute;n tay, l&amp;aacute; h&amp;igrave;nh dải, mũi m&amp;aacute;c, nhọn 2 đầu, d&amp;agrave;i tới 55cm, rộng 6cm mặt tr&amp;ecirc;n nhẵn, dưới c&amp;oacute; v&amp;agrave;i l&amp;ocirc;ng rải r&amp;aacute;c bẹ l&amp;aacute; nhẵn, c&amp;oacute; kh&amp;iacute;a, lưỡi bẹ rất ngắn. Cụm hoa mọc ở gốc của th&amp;acirc;n mang l&amp;aacute;, mọc b&amp;ograve;, d&amp;agrave;i khoảng 40cm, mảnh, nhẵn, bao bởi nhiều vảy chuyển dần th&amp;agrave;nh l&amp;aacute; bắc ở ph&amp;iacute;a tr&amp;ecirc;n, l&amp;aacute; bắc mau rụng. Cuống chung của cụm hoa ngắn, mang 3-5 hoa, ở n&amp;aacute;ch những l&amp;aacute; bắc nhỏ h&amp;igrave;nh tr&amp;aacute;i soan. Hoa m&amp;agrave;u trắng t&amp;iacute;m, c&amp;oacute; cuống ngắn, đ&amp;agrave;i h&amp;igrave;nh ống nhẵn, c&amp;oacute; 3 răng ngắn. Tr&amp;agrave;ng h&amp;igrave;nh ống nhẵn, d&amp;agrave;i hơn đ&amp;agrave;i 2 lần, th&amp;ugrave;y h&amp;igrave;nh tr&amp;aacute;i xoan t&amp;ugrave;, th&amp;ugrave;y giữa hơi d&amp;agrave;i rộng hơn, l&amp;otilde;m hơn. C&amp;aacute;nh m&amp;ocirc;i h&amp;igrave;nh thoi. Quả nang h&amp;igrave;nh trứng, bao bởi đ&amp;agrave;i tồn tại, c&amp;oacute; khi lớn đến 4cm.&lt;br /&gt;
+Dược liệu: Quả h&amp;igrave;nh cầu dẹt, c&amp;oacute; 3 m&amp;uacute;i, đường k&amp;iacute;nh 1 - 1,5 cm. Mặt ngo&amp;agrave;i vỏ m&amp;agrave;u trắng, c&amp;oacute; một số đường v&amp;acirc;n dọc, đ&amp;ocirc;i khi c&amp;ograve;n s&amp;oacute;t cuống quả. Vỏ quả kh&amp;ocirc; dễ t&amp;aacute;ch. Mỗi quả c&amp;oacute; 20 - 30 hạt, gọi l&amp;agrave; khấu mễ hoặc khấu nh&amp;acirc;n, tập hợp th&amp;agrave;nh khối h&amp;igrave;nh cầu gọi l&amp;agrave; khấu cầu. Khấu cầu chia l&amp;agrave;m 3 m&amp;uacute;i c&amp;oacute; m&amp;agrave;ng mỏng m&amp;agrave;u trắng ngăn c&amp;aacute;ch, mỗi m&amp;uacute;i c&amp;oacute; 7 - 10 hạt. H&amp;igrave;nh dạng hạt kh&amp;ocirc;ng đồng nhất, phần nhiều l&amp;agrave; h&amp;igrave;nh khối nhiều mặt kh&amp;ocirc;ng đều, đường k&amp;iacute;nh khoảng 3 mm, mặt ngo&amp;agrave;i m&amp;agrave;u n&amp;acirc;u nhạt đến n&amp;acirc;u thẫm, c&amp;oacute; v&amp;acirc;n nhỏ, chất cứng. Mặt cắt ngang m&amp;agrave;u trắng. Hạt chứa nhiều tinh dầu. M&amp;ugrave;i thơm, vị cay.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;5. Ph&amp;acirc;n bố:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;C&amp;acirc;y mọc hoang, được trồng ở nước ta v&amp;agrave; nhiều nước kh&amp;aacute;c.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;6. Trồng trọt:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;7. Bộ phận d&amp;ugrave;ng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Quả gần ch&amp;iacute;n phơi kh&amp;ocirc; của c&amp;acirc;y Bạch đậu khấu (Amomum cardamomum L.), họ Gừng (Zingiberaceae).&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;8. Thu h&amp;aacute;i, chế biến:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Thu h&amp;aacute;i v&amp;agrave;o m&amp;ugrave;a thu, h&amp;aacute;i c&amp;acirc;y tr&amp;ecirc;n 3 năm, h&amp;aacute;i quả c&amp;ograve;n giai đoạn xanh chuyển sang v&amp;agrave;ng xanh. H&amp;aacute;i về phơi trong r&amp;acirc;m cho kh&amp;ocirc;, c&amp;oacute; khi phơi kh&amp;ocirc; xong bỏ cuống rồi x&amp;ocirc;ng di&amp;ecirc;m sinh cho vỏ trắng cất d&amp;ugrave;ng, khi d&amp;ugrave;ng b&amp;oacute;c vỏ lấy hạt.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;H&amp;aacute;i quả khi c&amp;oacute; m&amp;agrave;u lục, bỏ cuống, phơi kh&amp;ocirc;. Khi d&amp;ugrave;ng bỏ vỏ quả lấy hạt, gi&amp;atilde; n&amp;aacute;t.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;9. Th&amp;agrave;nh phần ho&amp;aacute; học:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Tinh dầu trong đ&amp;oacute; th&amp;agrave;nh phần chủ yếu l&amp;agrave; borneol v&amp;agrave; camphor.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;10. C&amp;ocirc;ng năng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Ho&amp;aacute; thấp, h&amp;agrave;nh kh&amp;iacute;, ti&amp;ecirc;u bĩ, khai vị, ti&amp;ecirc;u thực, &amp;ocirc;n trung&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;11. C&amp;ocirc;ng dụng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Chữa đau bụng lạnh, đầy hơi, n&amp;ocirc;n oẹ, ăn kh&amp;ocirc;ng ti&amp;ecirc;u, ỉa chảy, tr&amp;uacute;ng độc rượu.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;12. C&amp;aacute;ch d&amp;ugrave;ng, liều lượng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Ng&amp;agrave;y 4-8g, dạng thuốc sắc hoặc bột.&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:21</t>
+  </si>
+  <si>
+    <t>Bạch linh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;strong&gt;1. T&amp;ecirc;n khoa học:&lt;/strong&gt;&amp;nbsp;Poria cocos Wolf.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;2. Họ:&lt;/strong&gt;&amp;nbsp;Nấm lỗ (Polyporaceae)&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;3. T&amp;ecirc;n kh&amp;aacute;c:&lt;/strong&gt;&amp;nbsp;Bạch linh, phục linh&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;4. M&amp;ocirc; tả:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Thể quả nấm Phục linh kh&amp;ocirc;: h&amp;igrave;nh cầu, h&amp;igrave;nh thoi, h&amp;igrave;nh cầu dẹt hoặc h&amp;igrave;nh khối kh&amp;ocirc;ng đều, lớn, nhỏ kh&amp;ocirc;ng đồng nhất, mặt ngo&amp;agrave;i m&amp;agrave;u n&amp;acirc;u đến n&amp;acirc;u đen, c&amp;oacute; nhiều vết nhăn r&amp;otilde; v&amp;agrave; lồi l&amp;otilde;m. Thể nặng, rắn chắc. Mặt bẻ sần s&amp;ugrave;i v&amp;agrave; c&amp;oacute; vết nứt, lớp viền ngo&amp;agrave;i m&amp;agrave;u n&amp;acirc;u nhạt, phần trong m&amp;agrave;u trắng, số &amp;iacute;t c&amp;oacute; m&amp;agrave;u hồng nhạt. C&amp;oacute; loại b&amp;ecirc;n trong c&amp;ograve;n mấy đoạn rễ th&amp;ocirc;ng (Phục thần). Nấm phục linh kh&amp;ocirc;ng m&amp;ugrave;i, vị nhạt, cắn d&amp;iacute;nh răng.&lt;/p&gt;
+&lt;p&gt;Phục linh b&amp;igrave;: L&amp;agrave; lớp ngo&amp;agrave;i Phục linh t&amp;aacute;ch ra, lớn, nhỏ, kh&amp;ocirc;ng đồng nhất. Mặt ngo&amp;agrave;i từ n&amp;acirc;u đến n&amp;acirc;u đen, mặt trong m&amp;agrave;u trắng hoặc n&amp;acirc;u nhạt. Chất tương đối xốp, hơi c&amp;oacute; t&amp;iacute;nh đ&amp;agrave;n hồi.&lt;/p&gt;
+&lt;p&gt;Phục linh khối: sau khi t&amp;aacute;ch lớp ngo&amp;agrave;i, phần c&amp;ograve;n lại được th&amp;aacute;i, cắt th&amp;agrave;nh phiến hay miếng, lớn nhỏ kh&amp;ocirc;ng đồng nhất, m&amp;agrave;u trắng, hồng nhạt hoặc n&amp;acirc;u nhạt.&lt;br /&gt;
+X&amp;iacute;ch phục linh: L&amp;agrave; lớp thứ hai sau lớp ngo&amp;agrave;i, hơi hồng hoặc n&amp;acirc;u nhạt.&lt;/p&gt;
+&lt;p&gt;Bạch phục linh: L&amp;agrave; phần b&amp;ecirc;n trong, m&amp;agrave;u trắng.&lt;/p&gt;
+&lt;p&gt;Phục thần: L&amp;agrave; phần nấm Phục linh &amp;ocirc;m đoạn rễ th&amp;ocirc;ng b&amp;ecirc;n trong.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;5. Ph&amp;acirc;n bố:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Một số rừng th&amp;ocirc;ng ở v&amp;ugrave;ng kh&amp;iacute; hậu m&amp;aacute;t của nước ta cũng c&amp;oacute; loại nấm n&amp;agrave;y nhưng chưa được nu&amp;ocirc;i trồng v&amp;agrave; khai th&amp;aacute;c, vị thuốc chủ yếu nhập từ Trung.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;6. Trồng trọt:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;7. Bộ phận d&amp;ugrave;ng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Dược liệu chia th&amp;agrave;nh 4 thứ:&lt;/p&gt;
+&lt;p&gt;Phục linh b&amp;igrave; l&amp;agrave; vỏ ngo&amp;agrave;i.&lt;/p&gt;
+&lt;p&gt;X&amp;iacute;ch phục linh l&amp;agrave; lớp thứ 2 sau vỏ ngo&amp;agrave;i.&lt;/p&gt;
+&lt;p&gt;Bạch phục linh l&amp;agrave; phần b&amp;ecirc;n trong m&amp;agrave;u trắng, thường được sơ chế th&amp;agrave;nh phiến h&amp;igrave;nh khối vu&amp;ocirc;ng dẹt.&lt;/p&gt;
+&lt;p&gt;Phục thần l&amp;agrave; những quả thể c&amp;oacute; l&amp;otilde;i gỗ (rễ th&amp;ocirc;ng) ở giữa.&lt;/p&gt;
+&lt;p&gt;Quốc.&lt;br /&gt;
+&lt;strong&gt;8.&amp;nbsp;&lt;/strong&gt;&lt;strong&gt;Thu h&amp;aacute;i, chế biến:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Thu hoạch từ th&amp;aacute;ng 7 đến th&amp;aacute;ng 9, loại bỏ đất c&amp;aacute;t, chất đống cho ra mồ h&amp;ocirc;i rồi rải ra chỗ tho&amp;aacute;ng gi&amp;oacute; cho se bề mặt, tiếp tục chất đống, ủ v&amp;agrave;i lần cho đến khi kh&amp;ocirc; nước v&amp;agrave; xuất hiện nhăn nheo bề mặt, phơi &amp;acirc;m can đến kh&amp;ocirc;. Hoặc Phục linh tươi th&amp;aacute;i miếng v&amp;agrave; phơi &amp;acirc;m can nơi tho&amp;aacute;ng gi&amp;oacute;. Tuỳ theo c&amp;aacute;c phần th&amp;aacute;i v&amp;agrave; m&amp;agrave;u sắc của Phục linh m&amp;agrave; c&amp;oacute; t&amp;ecirc;n gọi kh&amp;aacute;c nhau: Bạch phục linh, Phục linh b&amp;igrave;, X&amp;iacute;ch phục linh, Phục linh khối, Phục linh phiến.&lt;/p&gt;
+&lt;p&gt;Ng&amp;acirc;m Phục linh v&amp;agrave;o nước, rửa sạch, đồ th&amp;ecirc;m cho mềm, gọt vỏ, th&amp;aacute;i miếng hoặc th&amp;aacute;i l&amp;aacute;t l&amp;uacute;c đang mềm v&amp;agrave; phơi hoặc sấy kh&amp;ocirc;.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;9. Th&amp;agrave;nh phần ho&amp;aacute; học:&lt;/strong&gt;&amp;nbsp;đường (trong đ&amp;oacute; c&amp;oacute; pachymose l&amp;agrave; đường đặc hiệu), chất kho&amp;aacute;ng, c&amp;aacute;c hợp chất triterpenoid.&lt;/p&gt;
+&lt;p&gt;C&amp;ocirc;ng năng: thuốc lợi thuỷ v&amp;agrave; cường tr&amp;aacute;ng,&amp;nbsp; nhuận t&amp;aacute;o, bổ tỳ, &amp;iacute;ch kh&amp;iacute;&amp;ugrave;, sinh t&amp;acirc;n, chỉ kh&amp;aacute;t.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;10. T&amp;aacute;c dụng dược l&amp;yacute;:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Thuốc c&amp;oacute; t&amp;aacute;c dụng lợi tiểu, cũng c&amp;oacute; b&amp;aacute;o c&amp;aacute;o cho l&amp;agrave; t&amp;aacute;c dụng lợi tiểu kh&amp;ocirc;ng r&amp;otilde;, c&amp;oacute; thể do điều kiện nghi&amp;ecirc;n cứu kh&amp;aacute;c nhau.&lt;/p&gt;
+&lt;p&gt;Thuốc c&amp;oacute; t&amp;aacute;c dụng tăng miễn dịch, tăng chỉ số thực b&amp;agrave;o của phagocyte ở chuột.&amp;nbsp;&lt;br /&gt;
+Thuốc c&amp;oacute; t&amp;aacute;c dụng kh&amp;aacute;ng ung thư (do th&amp;agrave;nh phần polysacharide của thuốc) do l&amp;agrave;m tăng miễn dịch cơ thể.&lt;/p&gt;
+&lt;p&gt;Thuốc c&amp;oacute; t&amp;aacute;c dụng an thần, c&amp;oacute; t&amp;aacute;c dụng hạ đường huyết, bảo vệ gan v&amp;agrave; chống l&amp;oacute;et bao tử.&lt;/p&gt;
+&lt;p&gt;Nước sắc Phục linh c&amp;oacute; t&amp;aacute;c dụng ức chế đối với tụ cầu v&amp;agrave;ng, trực khuẩn đại tr&amp;agrave;ng, trực khuẩn biến dạng. Cồn ng&amp;acirc;m kiệt thuốc c&amp;oacute; t&amp;aacute;c dụng giết chết xoắn khuẩn.&lt;br /&gt;
+&lt;strong&gt;11.&amp;nbsp;&lt;/strong&gt;&lt;strong&gt;C&amp;ocirc;ng dụng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Phục linh b&amp;igrave;: Lợi tiểu, trị ph&amp;ugrave; thũng.&lt;/p&gt;
+&lt;p&gt;X&amp;iacute;ch phục linh: Chữa thấp nhiệt (chướng bụng, vi&amp;ecirc;m b&amp;agrave;ng quang, tiểu v&amp;agrave;ng, đ&amp;aacute;i rắt).&lt;/p&gt;
+&lt;p&gt;Bạch phục linh: Chữa ăn uống k&amp;eacute;m ti&amp;ecirc;u, đầy chướng, b&amp;iacute; tiểu tiện, ho c&amp;oacute; đờm, ỉa chảy.&lt;br /&gt;
+Phục thần: Trị yếu tim, hoảng sợ, hồi hộp, mất ngủ.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;12. C&amp;aacute;ch d&amp;ugrave;ng, liều lượng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Ng&amp;agrave;y 6-12g. Dạng thuốc sắc, ho&amp;agrave;n, t&amp;aacute;n. Phối hợp trong nhiều phương thuốc kh&amp;aacute;c nhau.&lt;/p&gt;
+&lt;p&gt;Ki&amp;ecirc;ng kỵ:&amp;nbsp;&amp;acirc;m hư m&amp;agrave; kh&amp;ocirc;ng thấp nhiệt th&amp;igrave; kh&amp;ocirc;ng n&amp;ecirc;n d&amp;ugrave;ng.&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:23</t>
+  </si>
+  <si>
+    <t>Bạch thược</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;strong&gt;1. T&amp;ecirc;n khoa học:&lt;/strong&gt;&amp;nbsp;Paeonia lactiflora Pall.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;2. Họ:&lt;/strong&gt;&amp;nbsp;Ho&amp;agrave;ng li&amp;ecirc;n (Ranunculaceae).&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;3. T&amp;ecirc;n kh&amp;aacute;c:&amp;nbsp;&lt;/strong&gt;Thược dược&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;4. M&amp;ocirc; tả:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;C&amp;acirc;y: C&amp;acirc;y thảo sống l&amp;acirc;u năm, cao 50-80cm, l&amp;aacute; mọc so le, chụm hai hay chụm ba, k&amp;eacute;p, với 9-12 phần ph&amp;acirc;n chia, c&amp;aacute;c đoạn kh&amp;ocirc;ng đều, h&amp;igrave;nh tr&amp;aacute;i xoan ngọn gi&amp;aacute;o, d&amp;agrave;i 8-12cm, rộng 2-4 cm m&amp;eacute;p nguy&amp;ecirc;n, ph&amp;iacute;a cuống hơi hồng. Hoa rất to mọc đơn độc, c&amp;oacute; m&amp;ugrave;i hoa Hồng, tr&amp;ecirc;n mỗi th&amp;acirc;n mang hoa c&amp;oacute; 1-7 hoa, rộng 10-12cm. Đ&amp;agrave;i c&amp;oacute; 6 phiến, c&amp;aacute;nh hoa xếp tr&amp;ecirc;n một d&amp;atilde;y hoặc hai d&amp;atilde;y, m&amp;agrave;u hồng thịt trước khi nở, rồi chuyển dần sang m&amp;agrave;u trắng tinh; bao phấn m&amp;agrave;u da cam. Quả gồm 3-5 l&amp;aacute; no&amp;atilde;n. C&amp;oacute; nhiều thứ trồng kh&amp;aacute;c nhau, c&amp;oacute; hoa c&amp;oacute; độ lớn, số lượng c&amp;aacute;nh hoa, m&amp;agrave;u sắc... kh&amp;aacute;c nhau. Hoa th&amp;aacute;ng 5-6.&lt;/p&gt;
+&lt;p&gt;Dược liệu : Rễ h&amp;igrave;nh trụ tr&amp;ograve;n, thẳng hoặc đ&amp;ocirc;i khi hơi uốn cong, hai đầu phẳng; đều nhau hoặc một đầu to hơn, d&amp;agrave;i 10 - 20 cm, đường k&amp;iacute;nh 1 - 2,0 cm. Mặt ngo&amp;agrave;i hơi trắng hoặc hồng nhạt, nhẵn hoặc đ&amp;ocirc;i khi c&amp;oacute; nếp nhăn dọc v&amp;agrave; vết t&amp;iacute;ch của rễ nhỏ. Đ&amp;ocirc;i khi c&amp;ograve;n vỏ ngo&amp;agrave;i m&amp;agrave;u n&amp;acirc;u thẫm. Chất rắn chắc, nặng, kh&amp;oacute; bẻ gẫy. Mặt cắt phẳng m&amp;agrave;u trắng ng&amp;agrave; hoặc hơi phớt hồng. M&amp;ocirc; mềm vỏ hẹp, mạch gỗ xếp th&amp;agrave;nh h&amp;igrave;nh nan hoa xe đạp, kh&amp;ocirc;ng c&amp;oacute; m&amp;ugrave;i, vị hơi đắng, hơi chua.&lt;br /&gt;
+Bộ phận d&amp;ugrave;ng : Vị thuốc l&amp;agrave; rễ đ&amp;atilde; cạo bỏ lớp bần v&amp;agrave; chế biến kh&amp;ocirc; của c&amp;acirc;y Thược dược (Paeonia lactiflora Pall.)&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;5. Ph&amp;acirc;n bố:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;C&amp;acirc;y được nhập giống từ Trung Quốc v&amp;agrave;o trồng ở Sapa (L&amp;agrave;o Cai). C&amp;acirc;y được trồng nơi n&amp;uacute;i cao, kh&amp;iacute; hậu m&amp;aacute;t, mọc dưới những c&amp;acirc;y bụi hoặc c&amp;acirc;y to.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;6. Trồng trọt:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;C&amp;oacute; khả năng ph&amp;aacute;t triển trồng ở c&amp;aacute;c v&amp;ugrave;ng chuy&amp;ecirc;n canh&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;7. Bộ phận d&amp;ugrave;ng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Củ.&amp;nbsp;D&amp;ugrave;ng loại củ c&amp;oacute; đường k&amp;iacute;nh 1-2cm, d&amp;agrave;i 10-15cm, m&amp;agrave;u trắng hồng, &amp;iacute;t xơ.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;8. Thu h&amp;aacute;i, chế biến:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Thu hoạch sau 4 năm, v&amp;agrave;o khoảng th&amp;aacute;ng 8-10. Đ&amp;agrave;o l&amp;ecirc;n, cắt bỏ th&amp;acirc;n rễ v&amp;agrave; rễ con, rửa sạch, ng&amp;acirc;m nước 1-2 giờ, ủ 1-2 ng&amp;agrave;y đ&amp;ecirc;m (c&amp;oacute; thể đồ), sau khi đồ sửa lại cho thẳng rồi phơi hay sấy kh&amp;ocirc;. C&amp;oacute; thể b&amp;agrave;o hay th&amp;aacute;i mỏng sau khi đồ rồi sao qua. C&amp;oacute; khi tẩm giấm rồi sao qua hay sao ch&amp;aacute;y cạnh, hoặc tẩm rượu sao qua. L&amp;uacute;c chưa b&amp;agrave;o chế cần phải sấy lưu huỳnh, sau khi b&amp;agrave;o chế cần để nơi kh&amp;ocirc; r&amp;aacute;o, tr&amp;aacute;nh ẩm.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;9. Th&amp;agrave;nh phần ho&amp;aacute; học:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Trong rễ c&amp;oacute; paeoniflorin, oxypaeoniflorin, albiflorin, benzoyl-paeoniflorin, oxypaeoniflorinone, paeonolide, paeonol... c&amp;ograve;n c&amp;oacute; tinh bột, tanin, calci oxalat, tinh dầu, chất b&amp;eacute;o, chất nhầy, acid benzoic.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;10. C&amp;ocirc;ng năng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Liễm &amp;acirc;m, dưỡng huyết, b&amp;igrave;nh can, chỉ thống&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;11. C&amp;ocirc;ng dụng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;D&amp;ugrave;ng dạng sống chữa nhức đầu, ch&amp;acirc;n tay đau nhức, trị tả lỵ, mồ h&amp;ocirc;i trộm, tiểu tiện kh&amp;oacute;, đ&amp;aacute;i đường; giải nhiệt, chữa cảm mạo do chứng lo g&amp;acirc;y n&amp;ecirc;n.&lt;/p&gt;
+&lt;p&gt;Dạng sao tẩm chữa c&amp;aacute;c bệnh về huyết, th&amp;ocirc;ng kinh nguyệt. Nếu sao ch&amp;aacute;y cạnh chữa băng huyết. Nếu sao v&amp;agrave;ng chữa đau bụng kinh, rong kinh&amp;hellip;&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;12. C&amp;aacute;ch d&amp;ugrave;ng, liều lượng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Ng&amp;agrave;y d&amp;ugrave;ng 6 -12g, dạng thuốc sắc.&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:24</t>
+  </si>
+  <si>
+    <t>Bạc hà</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;strong&gt;1. T&amp;ecirc;n khoa học&lt;/strong&gt;: Mentha arvensis L. (Bạc h&amp;agrave; &amp;Aacute;), hoặc Mentha piperita L. (Bạc h&amp;agrave; &amp;Acirc;u),&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;2. Họ:&amp;nbsp;&lt;/strong&gt;Bạc h&amp;agrave; (Lamiaceae). C&amp;acirc;y được trồng ở nhiều địa phương nước ta.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;3. T&amp;ecirc;n kh&amp;aacute;c:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;4. M&amp;ocirc; tả:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;C&amp;acirc;y thảo, sống l&amp;acirc;u năm. Th&amp;acirc;n mềm, h&amp;igrave;nh vu&amp;ocirc;ng. Loại th&amp;acirc;n ngầm mang rễ mọc b&amp;ograve; lan, loại th&amp;acirc;n đứng mang l&amp;aacute;, cao 30-40cm, c&amp;oacute; khi hơn, mầu xanh lục hoặc t&amp;iacute;m t&amp;iacute;a. L&amp;aacute; mọc đối, h&amp;igrave;nh bầu dục hoặc h&amp;igrave;nh trứng. Cuống ngắn. M&amp;eacute;p l&amp;aacute; kh&amp;iacute;a răng đều. Hoa nhỏ, mầu trắng, hồng hoặc t&amp;iacute;m hồng, mọc tụ tập ở kẽ l&amp;aacute; th&amp;agrave;nh những v&amp;ograve;ng nhiều hoa. L&amp;aacute; bắc nhỏ, h&amp;igrave;nh d&amp;ugrave;i. Đ&amp;agrave;i h&amp;igrave;nh chu&amp;ocirc;ng c&amp;oacute; 5 răng đều nhau. Tr&amp;agrave;ng c&amp;oacute; ống ngắn. Phiến tr&amp;agrave;ng chia l&amp;agrave;m 4 phần gần bằng nhau, c&amp;oacute; 1 v&amp;ograve;ng l&amp;ocirc;ng ở ph&amp;iacute;a trong. 4 nhụy bằng nhau, chi nhụy nhẵn. Quả bế c&amp;oacute; 4 hạt. C&amp;aacute;c bộ phận tr&amp;ecirc;n mặt đất c&amp;oacute; l&amp;ocirc;ng gồm l&amp;ocirc;ng che chở v&amp;agrave; l&amp;ocirc;ng b&amp;agrave;i tiết tinh dầu.&lt;/p&gt;
+&lt;p&gt;M&amp;ugrave;a hoa quả v&amp;agrave;o th&amp;aacute;ng 7 - 10.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;5. Ph&amp;acirc;n bố:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;C&amp;acirc;y của v&amp;ugrave;ng &amp;Acirc;u &amp;Aacute; &amp;ocirc;n đới. Ở nước ta c&amp;oacute; những c&amp;acirc;y mọc hoang ở miền n&amp;uacute;i, nơi đất ẩm, m&amp;aacute;t v&amp;agrave; những chủng nhập trồng ở nhiều nơi..&amp;nbsp;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;6. Trồng trọt:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;C&amp;acirc;y ưa đất xốp, tốt nhất l&amp;agrave; đất s&amp;eacute;t c&amp;oacute; nhiều m&amp;ugrave;n, ẩm ướt, tho&amp;aacute;t nước nhưng đủ độ ẩm. Đất cần l&amp;agrave;m cỏ b&amp;oacute;n ph&amp;acirc;n kỹ trước, l&amp;agrave;m luống rộng, tr&amp;ecirc;n mỗi luống trồng 2-3 h&amp;agrave;ng. C&amp;oacute; thể trồng quanh năm nhưng thường trồng v&amp;agrave;o 2 m&amp;ugrave;a l&amp;agrave; m&amp;ugrave;a xu&amp;acirc;n (th&amp;aacute;ng 2-3) v&amp;agrave; m&amp;ugrave;a thu (th&amp;aacute;ng 8-9), trồng v&amp;agrave;o m&amp;ugrave;a xu&amp;acirc;n cho năng suất cao nhất. Trồng bằng hạt (&amp;iacute;t &amp;aacute;p dụng), th&amp;acirc;n ngầm hoặc th&amp;acirc;n c&amp;acirc;y tr&amp;ecirc;n mặt đất, cắt đoạn d&amp;agrave;i 15-30cm. Sau 3-4 th&amp;aacute;ng c&amp;oacute; thể thu hoạch đợt đầu, thường một năm c&amp;oacute; thể cắt c&amp;acirc;y 3-4 lần; lần thứ nhất v&amp;agrave;o th&amp;aacute;ng 6-7, sau đ&amp;oacute; cần xới v&amp;agrave; b&amp;oacute;n ph&amp;acirc;n, sau 2 th&amp;aacute;ng (v&amp;agrave;o cuối th&amp;aacute;ng 8 hay th&amp;aacute;ng 9) lại h&amp;aacute;i lần nữa v&amp;agrave;o l&amp;uacute;c c&amp;acirc;y đang ra hoa nhiều. H&amp;aacute;i về, cần b&amp;oacute; lại từng b&amp;oacute;, phơi chỗ m&amp;aacute;t cho kh&amp;ocirc;, hoặc nếu cất tinh dầu th&amp;igrave; cần cất ngay hoặc để hơi h&amp;eacute;o rồi cất.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;7. Bộ phận d&amp;ugrave;ng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Th&amp;acirc;n, c&amp;agrave;nh mang l&amp;aacute; (Herba Menthae)&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;8. Thu h&amp;aacute;i, chế biến:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Thu h&amp;aacute;i v&amp;agrave;o khoảng th&amp;aacute;ng 5, 8, 11 thu hoạch l&amp;uacute;c c&amp;acirc;y mới ra hoa, rửa sạch d&amp;ugrave;ng tươi hoặc phơi trong r&amp;acirc;m cho kh&amp;ocirc;.&lt;/p&gt;
+&lt;p&gt;Lấy l&amp;aacute; Bạc h&amp;agrave; kh&amp;ocirc;, tẩm nước, để v&amp;agrave;o chỗ r&amp;acirc;m m&amp;aacute;t, khi l&amp;aacute; c&amp;acirc;y mềm, cắt ngắn từng đoạn, phơi trong r&amp;acirc;m cho kh&amp;ocirc; để d&amp;ugrave;ng (Trung Dược Đại Từ Điển).&lt;/p&gt;
+&lt;p&gt;Rửa qua, để r&amp;aacute;o nước, cắt ngắn chừng 2cm, phơi trong r&amp;acirc;m cho kh&amp;ocirc; (Dược Liệu Việt&amp;nbsp;Nam).&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;9. Th&amp;agrave;nh phần ho&amp;aacute; học ch&amp;iacute;nh:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Tinh dầu, trong đ&amp;oacute; th&amp;agrave;nh phần chủ yếu l&amp;agrave; menthol.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;10. T&amp;aacute;c dụng dược l&amp;yacute;:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;T&amp;aacute;c dụng kh&amp;aacute;ng khuẩn: nước sắc Bạc h&amp;agrave; c&amp;oacute; t&amp;aacute;c dụng ức chế đối với virus ECHO v&amp;agrave; Salmonella Typhoit (Trung Dược Học).&lt;/p&gt;
+&lt;p&gt;T&amp;aacute;c dụng tr&amp;ecirc;n cơ trơn: Menthol v&amp;agrave; Menthone c&amp;oacute; t&amp;aacute;c dụng ức chế tr&amp;ecirc;n ruột thỏ, Menthone c&amp;oacute; t&amp;aacute;c dụng mạnh hơn (Trung Dược Học).&lt;/p&gt;
+&lt;p&gt;Ức chế đau: Tinh dầu Bạc h&amp;agrave; v&amp;agrave; Menthol bốc hơi nhanh, g&amp;acirc;y cảm gi&amp;aacute;c m&amp;aacute;t v&amp;agrave; t&amp;ecirc; tại chỗ, d&amp;ugrave;ng trong trường hợp đau d&amp;acirc;y thần kinh (T&amp;agrave;i Nguy&amp;ecirc;n C&amp;acirc;y Thuốc Việt&amp;nbsp;Nam).&lt;/p&gt;
+&lt;p&gt;S&amp;aacute;t khuẩn mạnh: d&amp;ugrave;ng trong những trường hợp ngứa của 1 số bệnh ngo&amp;agrave;i da, bệnh về tai, mũi, họng (T&amp;agrave;i Nguy&amp;ecirc;n C&amp;acirc;y Thuốc Việt&amp;nbsp;Nam).&lt;/p&gt;
+&lt;p&gt;Ức chế h&amp;ocirc; hấp, tuần ho&amp;agrave;n: đối với trẻ em &amp;iacute;t tuổi, tinh dầu Bạc h&amp;agrave; v&amp;agrave; Menthol b&amp;ocirc;i v&amp;agrave;o mũi hoặc cổ họng c&amp;oacute; thể g&amp;acirc;y hiện tượng ức chế dẫn tới ngừng thở v&amp;agrave; tim ngưng đập ho&amp;agrave;n to&amp;agrave;n. Người ta đ&amp;atilde; nhận x&amp;eacute;t thấy 1 số trường hợp chết do nhỏ mũi 1 giọt dầu Menthol 1% hoặc b&amp;ocirc;i v&amp;agrave;o ni&amp;ecirc;m mạc mũi loại thuốc mỡ c&amp;oacute; Menthol. V&amp;igrave; vậy, cần hết sức thận trọng khi d&amp;ugrave;ng tinh dầu Bạc h&amp;agrave; hoặc dầu c&amp;ugrave; l&amp;agrave; cho trẻ nhỏ &amp;iacute;t tuổi, nhất l&amp;agrave; trẻ mới đẻ (T&amp;agrave;i Nguy&amp;ecirc;n C&amp;acirc;y Thuốc ViệtNam).&lt;/p&gt;
+&lt;p&gt;T&amp;aacute;c động đến nhiệt độ cơ thể: Bạc h&amp;agrave;, tinh dầu Bạc h&amp;agrave; hoặc Menthol uống với liều rất nhỏ c&amp;oacute; thể g&amp;acirc;y hưng phấn, l&amp;agrave;m tăng b&amp;agrave;i tiết của tuyến mồ h&amp;ocirc;i, l&amp;agrave;m nhiệt độ cơ thể hạ thấp (T&amp;agrave;i Nguy&amp;ecirc;n C&amp;acirc;y Thuốc Việt Nam).&lt;/p&gt;
+&lt;p&gt;Liều lớn c&amp;oacute; t&amp;aacute;c dụng k&amp;iacute;ch th&amp;iacute;ch tủy sống, g&amp;acirc;y t&amp;ecirc; liệt phản xạ v&amp;agrave; ngăn cản sự l&amp;ecirc;n men b&amp;igrave;nh thường trong ruột (T&amp;agrave;i Nguy&amp;ecirc;n C&amp;acirc;y Thuốc Việt&amp;nbsp;Nam).&lt;/p&gt;
+&lt;p&gt;Bạc h&amp;agrave; c&amp;oacute; t&amp;aacute;c dụng kh&amp;aacute;ng vi khuẩn trong th&amp;iacute; nghiệm In Vitro đối với c&amp;aacute;c chủng vi khuẩn tả Vibrio Choreia Elto, Vibrio Choreia Inaba, Vibrio Choreia Ogawa (T&amp;agrave;i Nguy&amp;ecirc;n C&amp;acirc;y Thuốc Việt&amp;nbsp;Nam).&lt;/p&gt;
+&lt;p&gt;Tinh dầu Bạc h&amp;agrave; c&amp;oacute; t&amp;aacute;c dụng ức chế thần kinh trung ương do t&amp;aacute;c dụng chủ yếu của Menthol (T&amp;agrave;i Nguy&amp;ecirc;n C&amp;acirc;y Thuốc Việt&amp;nbsp;Nam).&lt;/p&gt;
+&lt;p&gt;Tinh dầu Bạc h&amp;agrave; l&amp;agrave;m giảm sự vận động v&amp;agrave; chống co thắt của ruột non. C&amp;aacute;c chất Menthol v&amp;agrave; Menthone ức chế sự vận động của đường ti&amp;ecirc;u h&amp;oacute;a từ ruột xuống, c&amp;oacute; t&amp;aacute;c dụng l&amp;agrave;m gĩan mao mạch (T&amp;agrave;i Nguy&amp;ecirc;n C&amp;acirc;y Thuốc Việt&amp;nbsp;Nam).&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;11. C&amp;ocirc;ng năng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;T&amp;aacute;n phong nhiệt, hạ sốt, th&amp;ocirc;ng mũi, chữa nhức đầu, gi&amp;uacute;p ti&amp;ecirc;u h&amp;oacute;a, đau bụng&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;12. C&amp;ocirc;ng dụng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Chữa cảm c&amp;uacute;m, nhức đầu, ngạt mũi, vi&amp;ecirc;m họng, k&amp;iacute;ch th&amp;iacute;ch ti&amp;ecirc;u ho&amp;aacute;, chữa đau bụng, đầy bụng.&lt;/p&gt;
+&lt;p&gt;Cất tinh dầu bạc h&amp;agrave; v&amp;agrave; chế menthol d&amp;ugrave;ng để sản xuất dầu cao sao v&amp;agrave;ng, l&amp;agrave;m chất thơm cho c&amp;aacute;c sản phẩm thực phẩm như b&amp;aacute;nh kẹo, thuốc đ&amp;aacute;nh răng, v&amp;agrave; trong một số ng&amp;agrave;nh kỹ nghệ kh&amp;aacute;c.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;13. C&amp;aacute;ch d&amp;ugrave;ng, liều lượng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;D&amp;ugrave;ng dưới dạng thuốc x&amp;ocirc;ng, thuốc h&amp;atilde;m 12-20g mỗi ng&amp;agrave;y.&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>Ba kich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;strong&gt;1. T&amp;ecirc;n khoa học:&lt;/strong&gt;&amp;nbsp;Morinda officinalis How.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;2. Họ:&lt;/strong&gt;&amp;nbsp;C&amp;agrave; ph&amp;ecirc; - Rubiaceae.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;3. T&amp;ecirc;n kh&amp;aacute;c:&lt;/strong&gt;&amp;nbsp;D&amp;acirc;y ruột g&amp;agrave;, ba k&amp;iacute;ch thi&amp;ecirc;n, li&amp;ecirc;n ch&amp;acirc;u ba k&amp;iacute;ch, chẩu ph&amp;oacute;ng x&amp;igrave;, s&amp;aacute;y c&amp;aacute;y (Th&amp;aacute;i), thau t&amp;agrave;y c&amp;aacute;y (T&amp;agrave;y), chồi ho&amp;agrave;ng kim, ch&amp;agrave;y ki&amp;agrave;ng đ&amp;ograve;i (Dao).&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;4. M&amp;ocirc; tả thực vật:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;D&amp;acirc;y leo, sống nhiều năm, th&amp;acirc;n non m&amp;agrave;u t&amp;iacute;m, c&amp;oacute; l&amp;ocirc;ng, c&amp;agrave;nh non c&amp;oacute; cạnh. L&amp;aacute; mọc đối, cứng nhọn, h&amp;igrave;nh ngọn gi&amp;aacute;o thu&amp;ocirc;n d&amp;agrave;i 6-14cm, rộng 2,5-6cm, l&amp;uacute;c non m&amp;agrave;u xanh, c&amp;oacute; l&amp;ocirc;ng d&amp;agrave;i ở mặt dưới, sau đ&amp;oacute; &amp;iacute;t l&amp;ocirc;ng v&amp;agrave; c&amp;oacute; m&amp;agrave;u trắng mốc; l&amp;aacute; k&amp;egrave;m h&amp;igrave;nh ống. Hoa nhỏ, m&amp;agrave;u trắng sau hơi v&amp;agrave;ng, 2-10 c&amp;aacute;nh hoa, 4 nhị, mọc th&amp;agrave;nh cụm ở kẽ l&amp;aacute;, đầu c&amp;agrave;nh. Quả tr&amp;ograve;n, khi ch&amp;iacute;n m&amp;agrave;u đỏ. Tr&amp;aacute;nh nhầm với c&amp;acirc;y ba k&amp;iacute;ch l&amp;ocirc;ng (M. cochinchinensis DC.) v&amp;agrave; c&amp;acirc;y mặt quỷ (M. villosa Hook.).&lt;/p&gt;
+&lt;p&gt;M&amp;ugrave;a hoa: th&amp;aacute;ng 5-6, m&amp;ugrave;a quả: th&amp;aacute;ng 7-10.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;5. Ph&amp;acirc;n bố:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;C&amp;acirc;y mọc hoang ở v&amp;ugrave;ng rừng thứ sinh, trung du v&amp;agrave; miền n&amp;uacute;i c&amp;aacute;c tỉnh ph&amp;iacute;a Bắc, dưới t&amp;aacute;n một số kiểu rừng nhiệt đới ẩm l&amp;aacute; rộng thường xanh,nay trở n&amp;ecirc;n thứ sinh gồm c&amp;acirc;y bụi v&amp;agrave; d&amp;acirc;y leo chằng chịt hoặc ở bờ nương rẫy. Độ cao ph&amp;acirc;n bố khoảng 100m so với mặt biển. C&amp;agrave;ng l&amp;ecirc;n cao c&amp;acirc;y c&amp;agrave;ng thưa dần, đến độ cao khoảng 100m th&amp;igrave; hầu như hiếm gặp. C&amp;oacute; nhiều nhất ở c&amp;aacute; tỉnh Quảng Ninh, Ph&amp;uacute; Thọ, Ho&amp;agrave; B&amp;igrave;nh, H&amp;agrave; Giang, Lạng Sơn.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;6. Trồng trọt:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Ba k&amp;iacute;ch ưa s&amp;aacute;ng, ưa ẩm v&amp;agrave; chịu b&amp;oacute;ng, mọc tr&amp;ecirc;n đất feralit đỏ v&amp;agrave;ng, c&amp;oacute; lượng m&amp;ugrave;n ở mức trung b&amp;igrave;nh, tơi xốp v&amp;agrave; hơi chua, nhiệt độ kh&amp;ocirc;ng kh&amp;iacute; trung b&amp;igrave;nh năm khoảng 21-23oC.&lt;/p&gt;
+&lt;p&gt;Trồng bằng rễ, c&amp;agrave;nh b&amp;aacute;nh tẻ hay gieo ươm bằng hạt.&lt;/p&gt;
+&lt;p&gt;V&amp;agrave;o khoảng th&amp;aacute;ng 3-4, khi thời tiết ấm dần, chọn những c&amp;agrave;nh b&amp;aacute;nh tẻ ở c&amp;acirc;y Ba k&amp;iacute;ch sống khoẻ, chặt th&amp;agrave;nh từng đoạn 20-30cm, mỗi đoạn c&amp;oacute; 2-4 mắt. C&amp;oacute; thể đem trồng ngay hoặc gi&amp;acirc;m v&amp;agrave; vườn ươm cho đến khi nảy mầm, ra rễ mới đem trồng.&lt;/p&gt;
+&lt;p&gt;Chọn c&amp;aacute;c ruộng cao s&amp;aacute;t ch&amp;acirc;n n&amp;uacute;i hay đất nương rẫy đ&amp;atilde; ph&amp;aacute;t quang, đất c&amp;ograve;n m&amp;agrave;u mỡ, luon ẩm. Cuốc s&amp;acirc;u, để ải, l&amp;agrave;m nhỏ đất, đ&amp;aacute;nh luống cao 20-30cm, rộng 40cm nếu trồng th&amp;agrave;nh 1 h&amp;agrave;ng hoặc rộng hơn nếu trồng th&amp;agrave;nh 2 h&amp;agrave;ng. Tr&amp;ecirc;n luống cuốc th&amp;agrave;nh c&amp;aacute;c hố s&amp;acirc;u 15cm, c&amp;aacute;ch nhau 60cm (trồng được khoảng 30.000 kh&amp;oacute;m/ha). B&amp;oacute;n l&amp;oacute;t ph&amp;acirc;n chuồng mục (10 tấn/ha), trộn đều. Kh&amp;ocirc;ng d&amp;ugrave;ng ph&amp;acirc;n tươi v&amp;igrave; c&amp;oacute; thể l&amp;agrave;m thối rễ. Mặc d&amp;ugrave; Ba k&amp;iacute;ch l&amp;agrave; c&amp;acirc;y ưa s&amp;aacute;ng nhưng ở thời kỳ mới trồng, c&amp;acirc;y lại ưa b&amp;oacute;ng. V&amp;igrave; vậy cần l&amp;agrave;m gi&amp;agrave;n che cho từng luống, cao 0,7-1m, ở tr&amp;ecirc;n che bằng ph&amp;ecirc;n hay cỏ tranh, để lượng &amp;aacute;nh s&amp;aacute;ng lọt qua khoảng 50%.&lt;/p&gt;
+&lt;p&gt;Thời gian trồng th&amp;iacute;ch hợp từ th&amp;aacute;ng 3-4. Hom giống cắt xong đem xử l&amp;yacute; ngay, mỗi hốc 2-3 hom. Hom đặt nghi&amp;ecirc;ng lấp đất chặt chỉ để hở 1-3cm. Nếu khong c&amp;oacute; gi&amp;agrave;n che, đặt xong phải phủ ngay bằng c&amp;acirc;y tế, guột hoặc r&amp;aacute;c. Thường xuy&amp;ecirc;n tưới nước, giữ cho đất ẩm. Hom nảy mầm sau 10-15 ng&amp;agrave;y, tỷ lệ khoảng 60%.&lt;/p&gt;
+&lt;p&gt;Ba k&amp;iacute;ch sinh trưởng&amp;nbsp;&amp;nbsp;nhanh, chỉ sau 6-7 th&amp;aacute;ng trồng đ&amp;atilde; c&amp;oacute; thể vượt l&amp;ecirc;n tr&amp;ecirc;n gi&amp;agrave;n che, vươn l&amp;ecirc;n sống trong điều kiện chiếu s&amp;aacute;ng ho&amp;agrave;n to&amp;agrave;n. L&amp;uacute;c n&amp;agrave;y cần l&amp;agrave;m gi&amp;aacute; thể cho c&amp;acirc;y. Mỗi năm chỉ cần l&amp;agrave;m cỏ v&amp;agrave; vun xới 1 lần. V&amp;agrave;o thời kỳ hạn h&amp;aacute;n cần tưới th&amp;ecirc;m nước.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;7. Thu h&amp;aacute;i chế biến:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Ba k&amp;iacute;ch trồng được 3 năm c&amp;oacute; thể thu hoạch. Năng suất dược liệu l&amp;agrave; rễ phụ thuộc v&amp;agrave;o số năm trồng. Th&amp;ocirc;ng thường để nhiều năm, năng suất c&amp;agrave;ng cao. Thời gian thu hoạch thường v&amp;agrave;o th&amp;aacute;ng 10-11. Cũng c&amp;oacute; thể v&amp;agrave;o m&amp;ugrave;a xu&amp;acirc;n để tận dụng lấy giống trồng ngay.&lt;/p&gt;
+&lt;p&gt;D&amp;ugrave;ng cuốc đ&amp;agrave;o rộng xung quanh gốc, lấy to&amp;agrave;n bộ rễ, rửa sạch đất c&amp;aacute;t. Phơi nắng liền 6-7 ng&amp;agrave;y, sau đập nhẹ l&amp;agrave;m bẹt phần thịt rễ, tr&amp;aacute;nh đập mạnh l&amp;agrave;m n&amp;aacute;t rễ. Sau đ&amp;oacute; lại phơi đến kh&amp;ocirc;. Cắt th&amp;agrave;nh từng đoạn d&amp;agrave;i 10cm, r&amp;uacute;t bỏ l&amp;otilde;i, đựng trong bao c&amp;oacute;i. Để nơi kh&amp;ocirc; r&amp;aacute;o, tho&amp;aacute;ng gi&amp;oacute;, cần phải x&amp;ocirc;ng lưu huỳnh ngay trong kho để tr&amp;aacute;nh mốc mọt.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;8. Bộ phận d&amp;ugrave;ng:&lt;/strong&gt;&amp;nbsp;Rễ phơi hay sấy kh&amp;ocirc; của c&amp;acirc;y Ba k&amp;iacute;ch (Morinda officinalis How.), họ C&amp;agrave; ph&amp;ecirc; (Rubiaceae).&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;9. Th&amp;agrave;nh phần ho&amp;aacute; học:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Rễ tươi chứa chất đường, nhựa, acid hữu cơ, vitamin C, tinh dầu, anthraglycosid, phytosterol. Nhưng trong ba k&amp;iacute;ch kh&amp;ocirc; kh&amp;ocirc;ng thấy c&amp;oacute; vitamin C.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;10. T&amp;aacute;c dụng dược l&amp;yacute;:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;10.1. Tăng sức dẻo dai: Với phương ph&amp;aacute;p&amp;nbsp; chuột bơi, Ba K&amp;iacute;ch với liều 5-10g/kg d&amp;ugrave;ng li&amp;ecirc;n tiếp 7 ng&amp;agrave;y thấy c&amp;oacute; t&amp;aacute;c dụng tăng sức dẻo dai cho s&amp;uacute;c vật th&amp;iacute; nghiệm (Trung Dược Học).&lt;/p&gt;
+&lt;p&gt;10.2. Tăng&amp;nbsp; sức đề kh&amp;aacute;ng: d&amp;ugrave;ng phương ph&amp;aacute;p&amp;nbsp; g&amp;acirc;y nhiễm độc cấp bằng Ammoni Clorua tr&amp;ecirc;n chuột nhắt trắng, với liều 15g/kg, Ba K&amp;iacute;ch c&amp;oacute; t&amp;aacute;c dụng tăng cường sức đề kh&amp;aacute;ng chung của cơ thể đối với c&amp;aacute;c yếu tố độc hại (Trung Dược Học).&lt;/p&gt;
+&lt;p&gt;10.3. Chống vi&amp;ecirc;m: Tr&amp;ecirc;n m&amp;ocirc; h&amp;igrave;nh g&amp;acirc;y vi&amp;ecirc;m thực nghiệm ở chuột cống trắng bằng Kaolin với liều lượng 5-10g/kg, Ba K&amp;iacute;ch c&amp;oacute; t&amp;aacute;c dụng chống vi&amp;ecirc;m r&amp;otilde; rệt (Trung Dược Học).&lt;/p&gt;
+&lt;p&gt;10.4. Đối với hệ thống nội tiết: th&amp;iacute; nghiệm tr&amp;ecirc;n chuột lớn v&amp;agrave; chuột nhắt cho thấy Ba K&amp;iacute;ch kh&amp;ocirc;ng c&amp;oacute; t&amp;aacute;c dụng kiểu Androgen nhưng c&amp;oacute; thể c&amp;oacute; khả năng tăng cường hiệu lực của Androgen hoặc tăng cường qu&amp;aacute; tr&amp;igrave;nh chế tiết hormon Androgen (Trung Dược Học).&lt;/p&gt;
+&lt;p&gt;10.5. Nước sắc Ba K&amp;iacute;ch c&amp;oacute; t&amp;aacute;c dụng tương tự như ACTH l&amp;agrave;m cho tuyến ức chuột con bị teo (Trung Dược Học).&lt;/p&gt;
+&lt;p&gt;10.6. Nước sắc Ba K&amp;iacute;ch c&amp;oacute; t&amp;aacute;c dụng l&amp;agrave;m tăng co b&amp;oacute;p của chuột v&amp;agrave; hạ huyết &amp;aacute;p (Trung Dược Học).&lt;/p&gt;
+&lt;p&gt;10.7. Kh&amp;ocirc;ng c&amp;oacute; độc. LD50&amp;nbsp; của Ba K&amp;iacute;ch được x&amp;aacute;c định tr&amp;ecirc;n chuột nhắt trắng bằng đường uống l&amp;agrave; 193g/kg (Trung Dược Dược l&amp;yacute;, Độc l&amp;yacute; Dữ L&amp;acirc;m S&amp;agrave;ng).&lt;/p&gt;
+&lt;p&gt;Rễ Ba k&amp;iacute;ch chiết xuất bằng rượu c&amp;oacute; t&amp;aacute;c dụng gi&amp;aacute;ng &amp;aacute;p huyết; c&amp;oacute; t&amp;aacute;c dụng nhanh đối với c&amp;aacute;c tuyến cơ năng; tăng cường n&amp;atilde;o; chống ngủ ngon d&amp;ugrave;ng Ba k&amp;iacute;ch nhục (Trung Dược Dược l&amp;yacute;, Độc l&amp;yacute; Dữ L&amp;acirc;m S&amp;agrave;ng).&lt;/p&gt;
+&lt;p&gt;T&amp;aacute;c dụng đối với hệ nội tiết: Cho chuột v&amp;agrave; chuột nhắt uống Ba k&amp;iacute;ch thi&amp;ecirc;n thấy kh&amp;ocirc;ng c&amp;oacute; t&amp;aacute;c dụng giống như chất Androgen (Trung Dược Học).&lt;/p&gt;
+&lt;p&gt;Đối với những bệnh nh&amp;acirc;n nam c&amp;oacute; hoạt động sinh dục kh&amp;ocirc;ng b&amp;igrave;nh thường, Ba K&amp;iacute;ch c&amp;oacute; t&amp;aacute;c dụng l&amp;agrave;m tăng khả năng gioa hợp, đặc biệt đối với những trường hợp giao hợp yếu v&amp;agrave; thưa. Ba K&amp;iacute;ch c&amp;oacute; t&amp;aacute;c dụng tăng cường sức dẻo dai, mặc dầu n&amp;oacute; kh&amp;ocirc;ng l&amp;agrave;m tăng đ&amp;ograve;i hỏi t&amp;igrave;nh dục, kh&amp;ocirc;ng thấy c&amp;oacute; t&amp;aacute;c dụng kiểu Androgen. Tuy kh&amp;ocirc;ng l&amp;agrave;m thay đổi tinh dịch đồ nhưng tr&amp;ecirc;n thực tế c&amp;oacute; t&amp;aacute;c dụng hỗ trợ v&amp;agrave; cải thiện hoạt động sinh dục cũng như điều trị v&amp;ocirc; sinh cho những nam giới c&amp;oacute; trạng th&amp;aacute;i v&amp;ocirc; sinh tương đối v&amp;agrave; suy nhược thể lực. C&amp;ograve;n c&amp;aacute;c trường hợp tinh dịch &amp;iacute;t, tinh tr&amp;ugrave;ng chết nhiều, kh&amp;ocirc;ng c&amp;oacute; tinh tr&amp;ugrave;ng, kh&amp;ocirc;ng xuất tinh khi giao hợp th&amp;igrave; xử dụng Ba K&amp;iacute;ch chưa thấy kết quả (T&amp;agrave;i Nguy&amp;ecirc;n C&amp;acirc;y Thuốc ViệtNam).&lt;/p&gt;
+&lt;p&gt;Đối với cơ thể những người tuổi gi&amp;agrave;, những bệnh nh&amp;acirc;n kh&amp;ocirc;ng biểu hiện mệt mỏi, ăn k&amp;eacute;m, ngủ &amp;iacute;t, gầy yếu m&amp;agrave; kh&amp;ocirc;ng thấy c&amp;oacute; những yếu tố bệnh l&amp;yacute; g&amp;acirc;y n&amp;ecirc;n v&amp;agrave; 1 số trường hợp c&amp;oacute; đau mỏi c&amp;aacute;c khớp, Ba K&amp;iacute;ch c&amp;oacute; t&amp;aacute;c dụng tăng lực r&amp;otilde; rệt, thể hiện qua những cảmgi&amp;aacute;c chủ quan như đỡ mệt mỏi, ăn ngon, ngủ ngon v&amp;agrave; những dấu hiệu kh&amp;aacute;ch quan như tăng c&amp;acirc;n nặng, tăng cơ lực. C&amp;ograve;n đối với bệnh nh&amp;acirc;n đau mỏi c&amp;aacute;c khớp th&amp;igrave; sau khi d&amp;ugrave;ng Ba K&amp;iacute;ch d&amp;agrave;i ng&amp;agrave;y, c&amp;aacute;c triệu chứng đau mỏi giảm r&amp;otilde; rệt (T&amp;agrave;i Nguy&amp;ecirc;n C&amp;acirc;y Thuốc Việt&amp;nbsp;Nam).&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;11. C&amp;ocirc;ng năng:&lt;/strong&gt;&amp;nbsp;&amp;Ocirc;n thận, tr&amp;aacute;ng dương, cường tr&amp;aacute;ng c&amp;acirc;n cốt, khử phong thấp&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;12. C&amp;ocirc;ng dụng:&amp;nbsp;&lt;/strong&gt;Chữa liệt dương, di tinh, phụ nữ kh&amp;oacute; c&amp;oacute; thai, kinh nguyệt chậm, bế kinh, đau lưng mỏi gối...&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;13. C&amp;ocirc;ng dụng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Ba k&amp;iacute;ch dược d&amp;ugrave;ng chữa dương uỷ, phong thấp cước kh&amp;iacute;, g&amp;acirc;n cốt yếu mềm, lưng gối mỏi đau. Trong nh&amp;acirc;n d&amp;acirc;n, Ba k&amp;iacute;ch l&amp;agrave; vị thuốc&amp;nbsp;&amp;nbsp;c&amp;oacute; t&amp;aacute;c dụng bổ tr&amp;iacute; n&amp;atilde;o v&amp;agrave; tinh kh&amp;iacute;, chữa xuất tinh sớm, di mộng tinh, liệt dương, kinh nguyệt chậm hoặc bế kinh, phong thấp, huyết &amp;aacute;p cao.&lt;/p&gt;
+&lt;p&gt;Ng&amp;agrave;y d&amp;ugrave;ng 8-16 g, dạng thuốc sắc, cao lỏng, vi&amp;ecirc;n chế từ cao hoặc rượu thuốc. Người ta thường đ&amp;agrave;o củ c&amp;acirc;y mọc hoang về nấu với thịt g&amp;agrave; ăn hoặc ng&amp;acirc;m rượu uống để bồi bổ sức khoẻ.&lt;/p&gt;
+&lt;p&gt;Kh&amp;ocirc;ng d&amp;ugrave;ng khi rong kinh, kinh sớm. Người &amp;acirc;m hư qu&amp;aacute; vượng đại tiện t&amp;aacute;o kết kh&amp;ocirc;ng n&amp;ecirc;n d&amp;ugrave;ng.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;14. C&amp;aacute;ch d&amp;ugrave;ng, liều lượng:&lt;/strong&gt;&amp;nbsp;Ng&amp;agrave;y 8-16g dưới dạng thuốc sắc hay rượu thuốc. Phối hợp trong c&amp;aacute;c phương thuốc bổ thận.&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:25</t>
+  </si>
+  <si>
+    <t>Chè vằng khô</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Th&amp;agrave;nh phần: 100% ch&amp;egrave; vằng&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;&amp;nbsp;C&amp;ocirc;ng dụng:&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;- Thanh nhiệt, ti&amp;ecirc;u độc, lợi mật, lợi thấp, giảm đau nhức xương khớp&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;- Chống vi&amp;ecirc;m da, mụn nhọt, r&amp;ocirc;m sẩy, mẩn ngứa, giữ cho da mịn, sạch mụn&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;- kh&amp;aacute;ng vi&amp;ecirc;m, gi&amp;uacute;p lợi sữa, chống tắc sữa, vi&amp;ecirc;m tuyến vũ.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;&amp;nbsp;Đối tượng sử dụng:&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;-D&amp;ugrave;ng cho mọi đối tượng. Tốt cho phụ nữ sau khi sinh, &amp;iacute;t sữa, tắc sữa.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Hướng dẫn sử dụng:&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;-Lấy 20 - 30 g c&amp;ugrave;ng 1,5 &amp;ndash; 2l nướcđun s&amp;ocirc;i khoảng 5 ph&amp;uacute;t. Sử dụng l&amp;agrave;m thức uống hằng ng&amp;agrave;y cho gia đ&amp;igrave;nh, c&amp;oacute; thể uống n&amp;oacute;ng hoặc lạnh.&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:32</t>
+  </si>
+  <si>
+    <t>Bột trà xanh matcha Kyoto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Tr&amp;agrave; xanh chứa các ch&amp;acirc;́t&amp;nbsp; chống oxy ho&amp;aacute;, chống khuẩn, chống b&amp;eacute;o ph&amp;igrave;, hấp thụ Tannin v&amp;agrave; b&amp;agrave;i thải sắc tố đen trong cơ thể gi&amp;uacute;p da trắng, chống ung thư. Diệp lục trong trà xanh th&amp;uacute;c đẩy sự t&amp;aacute;i sinh của c&amp;aacute;c tổ chức v&amp;agrave; dịch m&amp;aacute;u, c&amp;aacute;c loại đường c&amp;oacute; thể tăng cường khả năng miễn dịch, Cafein gi&amp;uacute;p đầu &amp;oacute;c tỉnh t&amp;aacute;o, c&amp;oacute; t&amp;aacute;c dụng l&amp;agrave;m săn chắc da. Ngo&amp;agrave;i ra n&amp;oacute; c&amp;ograve;n chứa nhiều vitamin, kho&amp;aacute;ng chất, Axit Amin c&amp;oacute; chức năng điều tiết protein, gi&amp;uacute;p da tr&amp;agrave;n trề sức sống.&lt;br /&gt;
+&lt;br /&gt;
+&lt;strong&gt;CÁC C&amp;Ocirc;NG THỨC LÀM ĐẸP&lt;/strong&gt;&lt;br /&gt;
+&lt;br /&gt;
+- D&amp;ugrave;ng 1 th&amp;igrave;a c&amp;agrave; ph&amp;ecirc; b&amp;ocirc;̣t trà xanh đun s&amp;ocirc;i với 25ml nước, om trong 40 ph&amp;uacute;t rồi lọc lấy nước trong, để nguội, sau đ&amp;oacute; d&amp;ugrave;ng gạc mềm tẩm nước xoa đều l&amp;ecirc;n mặt v&amp;agrave; cổ trong mỗi buổi s&amp;aacute;ng v&amp;agrave; tối trước khi đi ngủ. C&amp;aacute;ch l&amp;agrave;m n&amp;agrave;y sẽ gi&amp;uacute;p da mặt bạn kh&amp;ocirc;ng bị sạm đen bởi &amp;aacute;nh nắng...&lt;br /&gt;
+&lt;br /&gt;
+- Trộn 100g mật ong với 2 th&amp;igrave;a c&amp;agrave; ph&amp;ecirc; nước ch&amp;egrave;, cũng d&amp;ugrave;ng gạc mềm tẩm dung dịch đắp l&amp;ecirc;n mặt từ 10-15 ph&amp;uacute;t, sau đ&amp;oacute; rửa lại bằng nước sạch. L&amp;agrave;m đều đặn 1 lần/ng&amp;agrave;y, bạn sẽ c&amp;oacute; 1 l&amp;agrave;n da mềm mại v&amp;agrave; tươi s&amp;aacute;ng.&lt;br /&gt;
+&lt;br /&gt;
+- D&amp;ugrave;ng 1 th&amp;igrave;a canh bột gạo khấy đều với b&amp;ocirc;̣t trà xanh và nước th&amp;agrave;nh 1 hỗn hợp nhuyễn rồi trộn với l&amp;ograve;ng đỏ trứng g&amp;agrave;. Xoa hỗn hợp l&amp;ecirc;n mặt 15-20 ph&amp;uacute;t, sau đ&amp;oacute; rửa bằng nước ấm. D&amp;ugrave;ng 1 lần/tuần, những nếp nhăn của bạn sẽ dần biến mất.&lt;br /&gt;
+&lt;br /&gt;
+- Trộn b&amp;ocirc;̣t trà xanh c&amp;ugrave;ng &amp;iacute;t kem tẩy tế b&amp;agrave;o chết cho da mặt hay cổ, duy tr&amp;igrave; một tuần hai lần. Hoạt chất trong tr&amp;agrave; sẽ lấy sạch bụi, kh&amp;aacute;ng khuẩn v&amp;agrave; đem lại cho da sự tươi mới, m&amp;aacute;t mẻ.&lt;br /&gt;
+&lt;br /&gt;
+- B&amp;ocirc;̣t trà xanh ho&amp;agrave; c&amp;ugrave;ng kem dưỡng thể rồi cho v&amp;agrave;o tủ lạnh để ngăn m&amp;aacute;t một l&amp;uacute;c. T&amp;aacute;c dụng của hỗn hợp n&amp;agrave;y l&amp;agrave; l&amp;agrave;m m&amp;aacute;t da v&amp;agrave; bổ sung dưỡng chất cho da.&lt;br /&gt;
+&lt;br /&gt;
+- Pha tr&amp;agrave; xanh v&amp;agrave;o nước n&amp;oacute;ng, đợi cho hơi n&amp;oacute;ng bốc đều lan toả, bạn gh&amp;eacute; mặt v&amp;agrave;o cốc tr&amp;agrave; đang kh&amp;oacute;i nhẹ nhắm mắt, h&amp;iacute;t thật s&amp;acirc;u hương vị cho tinh thần thư th&amp;aacute;i v&amp;agrave; để hơi tr&amp;agrave; x&amp;ocirc;ng mặt cho gi&amp;atilde;n nở lỗ ch&amp;acirc;n l&amp;ocirc;ng. Sau đ&amp;oacute;, thay bằng hỗn hợp tr&amp;agrave; xanh ho&amp;agrave; với kem dưỡng đ&amp;atilde; để tủ lạnh để b&amp;ocirc;i lại cho se lỗ ch&amp;acirc;n l&amp;ocirc;ng.&lt;br /&gt;
+- Trộn đều 1 th&amp;igrave;a bột tr&amp;agrave; xanh, 1 th&amp;igrave;a bạch chỉ, 2 th&amp;igrave;a bột đậu xanh, đắp k&amp;iacute;n l&amp;ecirc;n mặt khoảng khoảng 10 &amp;ndash; 15 ph&amp;uacute;t rồi d&amp;ugrave;ng nước lạnh rửa lại sẽ gi&amp;uacute;p l&amp;agrave;m sạch da, dưỡng v&amp;ugrave;ng da bị tổn thương do mụn.&lt;br /&gt;
+&lt;br /&gt;
+- Trộn đều 1 th&amp;igrave;a bột tr&amp;agrave; xanh, 1 th&amp;igrave;a bột m&amp;igrave;, 2 th&amp;igrave;a mật ong, sau đ&amp;oacute; rồi b&amp;ocirc;i lớp mỏng l&amp;ecirc;n mặt, ch&amp;uacute; &amp;yacute; cằm v&amp;agrave; cổ c&amp;oacute; thể b&amp;ocirc;i nhiều hơn một ch&amp;uacute;t. Để khoảng 20 &amp;ndash; 30 ph&amp;uacute;t rồi rửa lại bằng nước lạnh. N&amp;ecirc;n b&amp;ocirc;i mặt nạ n&amp;agrave;y l&amp;uacute;c vừa tắm xong l&amp;agrave; tốt hơn cả. Mặt nạ n&amp;agrave;y sẽ gi&amp;uacute;p da bạn tươi s&amp;aacute;ng hơn.&lt;br /&gt;
+&lt;br /&gt;
+- Tạo nước hoa hồng: 1 lạng bột tr&amp;agrave; xanh, nửa l&amp;iacute;t rượu nhẹ (dưới 10 độ).&lt;br /&gt;
+&lt;br /&gt;
+Cho cả hai thứ đ&amp;oacute; v&amp;agrave;o một b&amp;igrave;nh thật sạch, n&amp;uacute;t chặt lại v&amp;agrave; để v&amp;agrave;o chỗ m&amp;aacute;t. Khoảng 1 th&amp;aacute;ng sau lấy ra sử dụng, đảm bảo nước hoa hồng n&amp;agrave;y c&amp;ograve;n hiệu quả hơn so với c&amp;aacute;c mỹ phẩm th&amp;ocirc;ng thường.&lt;br /&gt;
+&amp;nbsp;&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:34</t>
+  </si>
+  <si>
+    <t>Hầu thủ FUSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;strong&gt;Hầu Thủ Fusi c&amp;oacute; c&amp;ocirc;ng dụng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;- Bồi bổ sức khỏe, tăng cường sức đề kh&amp;aacute;ng.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;- Hỗ trợ điều trị vi&amp;ecirc;m lo&amp;eacute;t dạ d&amp;agrave;y, t&amp;aacute; tr&amp;agrave;ng, vi&amp;ecirc;m lo&amp;eacute;t ruột&amp;hellip;&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;- C&amp;aacute;c bệnh về đường ti&amp;ecirc;u h&amp;oacute;a.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;- Hỗ trợ điều trị ung thư dạ d&amp;agrave;y, c&amp;aacute;c ung thư về ti&amp;ecirc;u h&amp;oacute;a&amp;hellip;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;C&amp;aacute;ch d&amp;ugrave;ng&lt;/strong&gt;: uống l&amp;uacute;c đ&amp;oacute;i&lt;/p&gt;
+&lt;p&gt;- Tăng sức đề kh&amp;aacute;ng, ph&amp;ograve;ng chống bệnh tật: Mỗi lần d&amp;ugrave;ng 2 vi&amp;ecirc;n, ng&amp;agrave;y d&amp;ugrave;ng 3 lần (s&amp;aacute;ng, trưa, tối)&lt;/p&gt;
+&lt;p&gt;- Hỗ trợ điều trị bệnh tật liều d&amp;ugrave;ng gấp đ&amp;ocirc;i&lt;/p&gt;
+&lt;p&gt;- Trẻ em liều d&amp;ugrave;ng bằng &amp;frac12; người lớn.&lt;/p&gt;
+&lt;p&gt;&lt;em&gt;Ch&amp;uacute; &amp;yacute;&lt;/em&gt;:&amp;nbsp;&lt;strong&gt;Hầu thủ Fusi kh&amp;ocirc;ng c&amp;oacute; t&amp;aacute;c dụng phụ.&lt;/strong&gt;&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:35</t>
+  </si>
+  <si>
+    <t>Vân chi FUSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;strong&gt;1. V&amp;acirc;n Chi Fusi c&amp;oacute; c&amp;ocirc;ng dụng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;- Hỗ trợ điều trị vi&amp;ecirc;m gan B.&lt;/p&gt;
+&lt;p&gt;- Hạn chế qu&amp;aacute; tr&amp;igrave;nh ph&amp;aacute;t triển của ung thư gan .&lt;/p&gt;
+&lt;p&gt;- Hỗ trợ điều trị ung thư đường h&amp;ocirc; hấp, ung thư v&amp;uacute;, ung thư tử cung, buồng trứng...&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;2. Nguồn gốc&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;V&amp;acirc;n Chi Fusi được thu h&amp;aacute;i v&amp;agrave; b&amp;agrave;o chế từ sợi thể (thể sợi) nấm V&amp;acirc;n chi.&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>Hồng chi FUSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;strong&gt;Hồng Chi Fusi c&amp;oacute; c&amp;ocirc;ng dụng:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;- Tăng cường sức khỏe, tăng khả năng miễn dịch của cơ thể.&lt;/p&gt;
+&lt;p&gt;- Gi&amp;uacute;p ổn định huyết &amp;aacute;p đối với bệnh nh&amp;acirc;n huyết &amp;aacute;p cao.&lt;/p&gt;
+&lt;p&gt;- Gi&amp;uacute;p giảm suy nhược thần kinh.&lt;/p&gt;
+&lt;p&gt;- Hỗ trợ hoạt động của tim mạch&lt;/p&gt;
+&lt;p&gt;- Hỗ trợ hoạt động của gan&lt;/p&gt;
+&lt;p&gt;- Hỗ trợ điều trị ung thư.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Liều lượng v&amp;agrave; c&amp;aacute;ch d&amp;ugrave;ng&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;- D&amp;ugrave;ng nước n&amp;oacute;ng (60-70độ C) để pha uống: b&amp;oacute;c g&amp;oacute;i Hồng chi FUSI đổ v&amp;agrave;o cốc sau đ&amp;oacute; đổ nước v&amp;agrave;o khuấy đều cho tan rồi uống hết.&lt;/p&gt;
+&lt;p&gt;- Hiệu quả của Linh chi tương đối chậm, khoảng 2-3 ng&amp;agrave;y mới c&amp;oacute; hiệu quả, c&amp;oacute; trường hợp 10-30 ng&amp;agrave;y nhưng hiệu quả ổn định, khi điều trị một bệnh n&amp;agrave;o đ&amp;oacute; l&amp;agrave;m thuy&amp;ecirc;n giảm c&amp;aacute;c bệnh kh&amp;aacute;c, điều trị một c&amp;aacute;ch tổng thể, n&amp;acirc;ng cao to&amp;agrave;n thể trạng v&amp;agrave; ph&amp;ograve;ng ngừa bệnh.&lt;/p&gt;
+&lt;p&gt;- D&amp;ugrave;ng cho người lớn 2 g&amp;oacute;i 1 ng&amp;agrave;y v&amp;agrave; trẻ em dưới 6 tuổi d&amp;ugrave;ng bằng &amp;frac12; người lớn. Trong trường hợp bị suy kiệt hay cần hỗ trợ sức khỏe nhanh th&amp;igrave; d&amp;ugrave;ng gấp đ&amp;ocirc;i.&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:36</t>
+  </si>
+  <si>
+    <t>Trùng thảo FUSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Đ&amp;ocirc;ng tr&amp;ugrave;ng hạ thảo l&amp;agrave; một dược liệu qu&amp;yacute; hiếm, m&amp;agrave; v&amp;agrave;o m&amp;ugrave;a đ&amp;ocirc;ng l&amp;agrave; con s&amp;acirc;u nhưng đến m&amp;ugrave;a hạ th&amp;igrave; th&amp;agrave;nh c&amp;acirc;y cỏ.Tại Trung Quốc, đ&amp;ocirc;ng tr&amp;ugrave;ng hạ thảo thường gặp ở v&amp;ugrave;ng rừng ẩm ướt tại c&amp;aacute;c tỉnh Tứ Xuy&amp;ecirc;n, V&amp;acirc;n Nam, T&amp;acirc;y Khang, T&amp;acirc;y Tạng.&lt;/p&gt;
+&lt;p&gt;Đ&amp;ocirc;ng tr&amp;ugrave;ng hạ thảo chứa protein (25 - 32%) một loại acid đặc biệt (acid cordycepic 1,3,4,5 - tetra - oxyhexahydrobenzoi) 7% v&amp;agrave; cordycepin.&lt;/p&gt;
+&lt;p&gt;Theo đ&amp;ocirc;ng y, đ&amp;ocirc;ng tr&amp;ugrave;ng hạ thảo vị ngọt, t&amp;iacute;nh &amp;ocirc;n, v&amp;agrave;o hai kinh phế v&amp;agrave; thận. N&amp;oacute; c&amp;oacute; t&amp;aacute;c dụng &amp;iacute;ch phế thận, cầm m&amp;aacute;u, ho&amp;aacute; đờm, d&amp;ugrave;ng chữa hư lao sinh ho, ho ra m&amp;aacute;u, yếu sinh l&amp;yacute;. Ngo&amp;agrave;i ra Đ&amp;ocirc;ng tr&amp;ugrave;ng hạ thảo c&amp;oacute; thể d&amp;ugrave;ng để điều trị bệnh vi&amp;ecirc;m phế quản m&amp;atilde;n tĩnh v&amp;agrave; hen phế quản rất tốt.&lt;/p&gt;
+&lt;p&gt;Tr&amp;ugrave;ng thảo Fusi được thu h&amp;aacute;i v&amp;agrave; b&amp;agrave;o chế từ 100% sợi thể (thể sợi) đ&amp;ocirc;ng tr&amp;ugrave;ng hạ thảo bằng phương ph&amp;aacute;p sinh học hiện đại, m&amp;agrave; kh&amp;ocirc;ng c&amp;oacute; th&amp;ecirc;m bất cứ một t&amp;aacute; dược n&amp;agrave;o kh&amp;aacute;c. Sợi thể Đ&amp;ocirc;ng tr&amp;ugrave;ng hạ thảo chứa tất cả c&amp;aacute;c axitamin, vitamin B1, B2, B12, E v&amp;agrave; K, một loạt c&amp;aacute;c loại đường bao gồm mono-di v&amp;agrave; Si, Ni,&amp;hellip;v&amp;agrave; rất nhiều Polysaccharids(rất đa dạng v&amp;agrave; phức tạp), Protein, Sterol, Nucleosides v&amp;agrave; c&amp;aacute;c chất v&amp;ocirc; cơ: K, Na, Ca. Ngo&amp;agrave;i ra, sợi thể Đ&amp;ocirc;ng tr&amp;ugrave;ng hạ thảo c&amp;ograve;n chứa 28 axit b&amp;eacute;o no v&amp;agrave; chưa no trong đ&amp;oacute; đặc biệt c&amp;oacute; c&amp;aacute;c axit b&amp;eacute;o chưa no c&amp;oacute; t&amp;aacute;c dụng chống oxy h&amp;oacute;a như acidlinoleic&amp;hellip;chiếm 82%.&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:37</t>
+  </si>
+  <si>
+    <t>Hà thủ ô</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;H&amp;atilde;ng sản xuất : Nguyễn Th&amp;aacute;i Trang&lt;br /&gt;
+C&amp;ocirc;ng dụng : Tr&amp;agrave; được chế biến từ củ H&amp;Agrave; THỦ &amp;Ocirc;, c&amp;ograve;n c&amp;oacute; t&amp;ecirc;n l&amp;agrave; DẠ GIAO ĐẰNG ( v&amp;igrave; ban đ&amp;ecirc;m hai th&amp;acirc;n d&amp;acirc;y quấn lại v&amp;agrave;o nhau ) . T&amp;ecirc;n khoa học : Polygonum Multiflorum .&lt;br /&gt;
+- H&amp;agrave; Thủ &amp;Ocirc; l&amp;agrave; một loại dựoc liệu qu&amp;yacute; sống thi&amp;ecirc;n nhi&amp;ecirc;n, trong d&amp;acirc;n gian d&amp;ugrave;ng l&amp;agrave;m thuốc bổ m&amp;aacute;u, trị thần kinh suy nhược, kh&amp;oacute; ngủ. D&amp;ugrave;ng l&amp;acirc;u bổ gan thận , dưỡng huyết , &amp;iacute;ch tinh, mạnh g&amp;acirc;n cốt, sống l&amp;acirc;u.L&amp;agrave;m đen t&amp;oacute;c, tr&amp;aacute;nh rụng t&amp;oacute;c, bồi bổ cơ thể, đem lại thanh xu&amp;acirc;n cho mọi người&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:39</t>
+  </si>
+  <si>
+    <t>Trà linh chi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Tr&amp;agrave; linh chi c&amp;oacute; ưu điểm l&amp;agrave; điều chế đơn giản, sử dụng thuận tiện, kh&amp;ocirc;ng phải đun nấu cầu kỳ như thuốc sắc. Người ta thường chọn mua loại nấm to, l&amp;agrave;nh lặn, dầy dặn v&amp;agrave; c&amp;ograve;n nguy&amp;ecirc;n t&amp;aacute;n.&lt;br /&gt;
+&lt;br /&gt;
+Sau c&amp;ocirc;ng đoạn l&amp;agrave;m sạch, d&amp;ugrave;ng dao th&amp;aacute;i vụn hoặc th&amp;aacute;i th&amp;agrave;nh l&amp;aacute;t mỏng, c&amp;agrave;ng vụn c&amp;agrave;ng mỏng th&amp;igrave; c&amp;agrave;ng tốt v&amp;igrave; như vậy khi h&amp;atilde;m với nước s&amp;ocirc;i mới chiết xuất được tối đa hoạt chất.&lt;br /&gt;
+&lt;br /&gt;
+Cuối c&amp;ugrave;ng đem sấy hoặc phơi thật kh&amp;ocirc; rồi đựng trong lọ k&amp;iacute;n d&amp;ugrave;ng dần. Cũng c&amp;oacute; thể d&amp;ugrave;ng m&amp;aacute;y t&amp;aacute;n th&amp;agrave;nh dạng mịn như b&amp;ocirc;ng, c&amp;aacute;ch n&amp;agrave;y gi&amp;uacute;p người ta sau khi h&amp;atilde;m vừa uống được nước vừa ăn cả b&amp;atilde; một c&amp;aacute;ch dễ d&amp;agrave;ng v&amp;agrave; tiết kiệm.&lt;br /&gt;
+H&amp;atilde;ng sản xuất Ganoderma&lt;br /&gt;
+Xuất xứ: Bắc Triều Ti&amp;ecirc;n&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:40</t>
+  </si>
+  <si>
+    <t>Hồng sâm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Quy c&amp;aacute;ch&lt;br /&gt;
+-T&amp;ecirc;n gọi: Tr&amp;agrave; Hồng S&amp;acirc;m, Korean Red Ginseng Tea&lt;br /&gt;
+- Trọng lượng: 300gr / 100 g&amp;oacute;i&lt;br /&gt;
+- Dạng th&amp;agrave;nh phẩm: hộp gỗ&lt;br /&gt;
+&lt;br /&gt;
+&lt;strong&gt;C&amp;ocirc;ng Dụng:&lt;/strong&gt;&lt;br /&gt;
+-Ph&amp;ograve;ng chống ung thư, tốt cho gan, thận, điều h&amp;ograve;a huyết &amp;aacute;p vừa c&amp;oacute; khả năng dự ph&amp;ograve;ng t&amp;iacute;ch cực c&amp;aacute;c biến chứng tim mạch thường c&amp;oacute; tr&amp;ecirc;n bệnh nh&amp;acirc;n bị bệnh tiểu đường, đặc biệt l&amp;agrave; t&amp;igrave;nh trạng vi&amp;ecirc;m tắc động tĩnh mạch.&lt;br /&gt;
+-Bổ gan, thận, giải độc.&lt;br /&gt;
+-Vi&amp;ecirc;m gan cấp v&amp;agrave; m&amp;atilde;n t&amp;iacute;nh, gan nhiễm mỡ.&lt;br /&gt;
+-Vi&amp;ecirc;m gan si&amp;ecirc;u vi A+B c&amp;aacute;c loại.&lt;br /&gt;
+&lt;br /&gt;
+&lt;strong&gt;Xuất xứ&lt;/strong&gt;&amp;nbsp;&lt;strong&gt;:&lt;/strong&gt;&amp;nbsp;H&amp;agrave;n Quốc&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>01/12/2016 17:42</t>
   </si>
 </sst>
 </file>
@@ -808,7 +1431,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1326,6 +1949,806 @@
       </c>
       <c r="J16">
         <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17">
+        <v>88000</v>
+      </c>
+      <c r="D17">
+        <v>200</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18">
+        <v>78000</v>
+      </c>
+      <c r="D18">
+        <v>200</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19">
+        <v>158000</v>
+      </c>
+      <c r="D19">
+        <v>200</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20">
+        <v>128000</v>
+      </c>
+      <c r="D20">
+        <v>200</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21">
+        <v>60000</v>
+      </c>
+      <c r="D21">
+        <v>200</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22">
+        <v>90000</v>
+      </c>
+      <c r="D22">
+        <v>200</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23">
+        <v>50000</v>
+      </c>
+      <c r="D23">
+        <v>200</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" t="s">
+        <v>75</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24">
+        <v>85000</v>
+      </c>
+      <c r="D24">
+        <v>200</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25">
+        <v>130000</v>
+      </c>
+      <c r="D25">
+        <v>200</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" t="s">
+        <v>81</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26">
+        <v>108000</v>
+      </c>
+      <c r="D26">
+        <v>200</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>83</v>
+      </c>
+      <c r="G26" t="s">
+        <v>84</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27">
+        <v>78000</v>
+      </c>
+      <c r="D27">
+        <v>200</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>86</v>
+      </c>
+      <c r="G27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28">
+        <v>88000</v>
+      </c>
+      <c r="D28">
+        <v>200</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" t="s">
+        <v>90</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29">
+        <v>178000</v>
+      </c>
+      <c r="D29">
+        <v>200</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" t="s">
+        <v>93</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30">
+        <v>98000</v>
+      </c>
+      <c r="D30">
+        <v>200</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>95</v>
+      </c>
+      <c r="G30" t="s">
+        <v>96</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31">
+        <v>148000</v>
+      </c>
+      <c r="D31">
+        <v>200</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>98</v>
+      </c>
+      <c r="G31" t="s">
+        <v>96</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32">
+        <v>68000</v>
+      </c>
+      <c r="D32">
+        <v>200</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G32" t="s">
+        <v>101</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33">
+        <v>98000</v>
+      </c>
+      <c r="D33">
+        <v>200</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>103</v>
+      </c>
+      <c r="G33" t="s">
+        <v>104</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34">
+        <v>190000</v>
+      </c>
+      <c r="D34">
+        <v>200</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>106</v>
+      </c>
+      <c r="G34" t="s">
+        <v>107</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35">
+        <v>536000</v>
+      </c>
+      <c r="D35">
+        <v>200</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G35" t="s">
+        <v>110</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36">
+        <v>586000</v>
+      </c>
+      <c r="D36">
+        <v>200</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>112</v>
+      </c>
+      <c r="G36" t="s">
+        <v>110</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37">
+        <v>286000</v>
+      </c>
+      <c r="D37">
+        <v>200</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>114</v>
+      </c>
+      <c r="G37" t="s">
+        <v>115</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38">
+        <v>986000</v>
+      </c>
+      <c r="D38">
+        <v>200</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>117</v>
+      </c>
+      <c r="G38" t="s">
+        <v>118</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39">
+        <v>38000</v>
+      </c>
+      <c r="D39">
+        <v>200</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>120</v>
+      </c>
+      <c r="G39" t="s">
+        <v>121</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>122</v>
+      </c>
+      <c r="C40">
+        <v>133000</v>
+      </c>
+      <c r="D40">
+        <v>200</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>123</v>
+      </c>
+      <c r="G40" t="s">
+        <v>124</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>125</v>
+      </c>
+      <c r="C41">
+        <v>200000</v>
+      </c>
+      <c r="D41">
+        <v>200</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41" t="s">
+        <v>126</v>
+      </c>
+      <c r="G41" t="s">
+        <v>127</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Salesmanager] Edit Product - Fixbug
</commit_message>
<xml_diff>
--- a/assets/export/product.xlsx
+++ b/assets/export/product.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="132">
   <si>
     <t>Mã sản phẩm</t>
   </si>
@@ -1105,25 +1105,6 @@
   </si>
   <si>
     <t>01/12/2016 17:42</t>
-  </si>
-  <si>
-    <t>sản phẩm mới 1214</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;chưa biết m&amp;ocirc; tả thế n&amp;agrave;o&lt;/p&gt;
-</t>
-  </si>
-  <si>
-    <t>13/12/2016 00:15</t>
-  </si>
-  <si>
-    <t>thêm cái nữa lúc 1233</t>
-  </si>
-  <si>
-    <t>Mô tả thế nào đó</t>
-  </si>
-  <si>
-    <t>13/12/2016 00:34</t>
   </si>
 </sst>
 </file>
@@ -1462,7 +1443,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1516,7 +1497,7 @@
         <v>78000</v>
       </c>
       <c r="D2">
-        <v>50</v>
+        <v>189</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -2003,7 +1984,7 @@
         <v>56</v>
       </c>
       <c r="C16">
-        <v>1000</v>
+        <v>148000</v>
       </c>
       <c r="D16">
         <v>190</v>
@@ -2843,10 +2824,10 @@
         <v>126</v>
       </c>
       <c r="C40">
-        <v>133000</v>
+        <v>25000</v>
       </c>
       <c r="D40">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
@@ -2864,7 +2845,7 @@
         <v>0</v>
       </c>
       <c r="J40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K40">
         <v>1</v>
@@ -2878,10 +2859,10 @@
         <v>129</v>
       </c>
       <c r="C41">
-        <v>200000</v>
+        <v>70000</v>
       </c>
       <c r="D41">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="E41" t="s">
         <v>19</v>
@@ -2899,79 +2880,9 @@
         <v>0</v>
       </c>
       <c r="J41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>132</v>
-      </c>
-      <c r="C42">
-        <v>33000</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42" t="s">
-        <v>50</v>
-      </c>
-      <c r="F42" t="s">
-        <v>133</v>
-      </c>
-      <c r="G42" t="s">
-        <v>134</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="J42">
-        <v>0</v>
-      </c>
-      <c r="K42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>135</v>
-      </c>
-      <c r="C43">
-        <v>123456</v>
-      </c>
-      <c r="D43">
-        <v>3</v>
-      </c>
-      <c r="E43" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" t="s">
-        <v>136</v>
-      </c>
-      <c r="G43" t="s">
-        <v>137</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
-        <v>0</v>
-      </c>
-      <c r="K43">
         <v>1</v>
       </c>
     </row>

</xml_diff>